<commit_message>
Save funciton testing and working
</commit_message>
<xml_diff>
--- a/Figuring out DMAB c.xlsx
+++ b/Figuring out DMAB c.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
   <si>
     <t>total play count</t>
   </si>
@@ -88,13 +89,37 @@
   <si>
     <t>under the sqrt sign</t>
   </si>
+  <si>
+    <t>instant reward</t>
+  </si>
+  <si>
+    <t>average reward</t>
+  </si>
+  <si>
+    <t>avg dev</t>
+  </si>
+  <si>
+    <t>max dev</t>
+  </si>
+  <si>
+    <t>avg - max</t>
+  </si>
+  <si>
+    <t>playcount</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -140,14 +165,25 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -426,7 +462,7 @@
   <dimension ref="A1:AI47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,7 +475,7 @@
         <v>17</v>
       </c>
       <c r="B1">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -562,14 +598,14 @@
         <v>1.0009999999999999</v>
       </c>
       <c r="B4">
-        <f>T4*$B$1+$E$1</f>
-        <v>0.40624723500386212</v>
+        <f t="shared" ref="B4:B23" si="0">T4*$B$1+$E$1</f>
+        <v>0.40416482333590809</v>
       </c>
       <c r="S4">
         <v>1.0009999999999999</v>
       </c>
       <c r="T4" s="1">
-        <f>SQRT(LOG(S4)/1.001)</f>
+        <f t="shared" ref="T4:T23" si="1">SQRT(LOG(S4)/1.001)</f>
         <v>2.082411667954033E-2</v>
       </c>
       <c r="U4" s="1"/>
@@ -588,22 +624,22 @@
         <v>2.0009999999999999</v>
       </c>
       <c r="B5">
-        <f>T5*$B$1+$E$1</f>
-        <v>0.56457567506905326</v>
+        <f t="shared" si="0"/>
+        <v>0.50971711671270215</v>
       </c>
       <c r="C5">
-        <f>U5*$B$1+$E$1</f>
-        <v>0.51640165083224243</v>
+        <f t="shared" ref="C5:C23" si="2">U5*$B$1+$E$1</f>
+        <v>0.4776011005548283</v>
       </c>
       <c r="S5">
         <v>2.0009999999999999</v>
       </c>
       <c r="T5" s="1">
-        <f>SQRT(LOG(S5)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>0.54858558356351073</v>
       </c>
       <c r="U5" s="1">
-        <f t="shared" ref="U5:U23" si="0">SQRT(LOG(S5)/2.001)</f>
+        <f t="shared" ref="U5:U23" si="3">SQRT(LOG(S5)/2.001)</f>
         <v>0.38800550277414131</v>
       </c>
       <c r="V5" s="1"/>
@@ -621,30 +657,30 @@
         <v>3.0009999999999999</v>
       </c>
       <c r="B6">
-        <f>T6*$B$1+$E$1</f>
-        <v>0.60714977325519104</v>
+        <f t="shared" si="0"/>
+        <v>0.53809984883679407</v>
       </c>
       <c r="C6">
-        <f>U6*$B$1+$E$1</f>
-        <v>0.5465136057701826</v>
+        <f t="shared" si="2"/>
+        <v>0.49767573718012176</v>
       </c>
       <c r="D6">
-        <f>V6*$B$1+$E$1</f>
-        <v>0.51963782342197584</v>
+        <f t="shared" ref="D6:D23" si="4">V6*$B$1+$E$1</f>
+        <v>0.47975854894798392</v>
       </c>
       <c r="S6">
         <v>3.0009999999999999</v>
       </c>
       <c r="T6" s="1">
-        <f>SQRT(LOG(S6)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>0.69049924418397013</v>
       </c>
       <c r="U6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.48837868590060857</v>
       </c>
       <c r="V6" s="1">
-        <f t="shared" ref="V5:V23" si="1">SQRT(LOG(S6)/3.001)</f>
+        <f t="shared" ref="V6:V23" si="5">SQRT(LOG(S6)/3.001)</f>
         <v>0.39879274473991938</v>
       </c>
       <c r="W6" s="1"/>
@@ -661,38 +697,38 @@
         <v>4.0010000000000003</v>
       </c>
       <c r="B7">
-        <f>T7*$B$1+$E$1</f>
-        <v>0.63268224813146845</v>
+        <f t="shared" si="0"/>
+        <v>0.55512149875431227</v>
       </c>
       <c r="C7">
-        <f>U7*$B$1+$E$1</f>
-        <v>0.56457230262307068</v>
+        <f t="shared" si="2"/>
+        <v>0.5097148684153805</v>
       </c>
       <c r="D7">
-        <f>V7*$B$1+$E$1</f>
-        <v>0.5343839159364534</v>
+        <f t="shared" si="4"/>
+        <v>0.48958927729096896</v>
       </c>
       <c r="E7">
-        <f>W7*$B$1+$E$1</f>
-        <v>0.51638473290992171</v>
+        <f t="shared" ref="E7:E23" si="6">W7*$B$1+$E$1</f>
+        <v>0.47758982193994781</v>
       </c>
       <c r="S7">
         <v>4.0010000000000003</v>
       </c>
       <c r="T7" s="1">
-        <f>SQRT(LOG(S7)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>0.77560749377156135</v>
       </c>
       <c r="U7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.54857434207690214</v>
       </c>
       <c r="V7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.44794638645484469</v>
       </c>
       <c r="W7" s="1">
-        <f t="shared" ref="W5:W23" si="2">SQRT(LOG(S7)/4.001)</f>
+        <f t="shared" ref="W7:W23" si="7">SQRT(LOG(S7)/4.001)</f>
         <v>0.38794910969973895</v>
       </c>
       <c r="X7" s="1"/>
@@ -708,46 +744,46 @@
         <v>5.0010000000000003</v>
       </c>
       <c r="B8">
-        <f>T8*$B$1+$E$1</f>
-        <v>0.65070353935404557</v>
+        <f t="shared" si="0"/>
+        <v>0.56713569290269705</v>
       </c>
       <c r="C8">
-        <f>U8*$B$1+$E$1</f>
-        <v>0.57731846360680295</v>
+        <f t="shared" si="2"/>
+        <v>0.51821230907120208</v>
       </c>
       <c r="D8">
-        <f>V8*$B$1+$E$1</f>
-        <v>0.54479197974092908</v>
+        <f t="shared" si="4"/>
+        <v>0.49652798649395269</v>
       </c>
       <c r="E8">
-        <f>W8*$B$1+$E$1</f>
-        <v>0.52539875603577058</v>
+        <f t="shared" si="6"/>
+        <v>0.48359917069051372</v>
       </c>
       <c r="F8">
-        <f>X8*$B$1+$E$1</f>
-        <v>0.5121628605216626</v>
+        <f t="shared" ref="F8:F23" si="8">X8*$B$1+$E$1</f>
+        <v>0.47477524034777507</v>
       </c>
       <c r="S8">
         <v>5.0010000000000003</v>
       </c>
       <c r="T8" s="1">
-        <f>SQRT(LOG(S8)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>0.83567846451348515</v>
       </c>
       <c r="U8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.59106154535600997</v>
       </c>
       <c r="V8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.48263993246976344</v>
       </c>
       <c r="W8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.4179958534525684</v>
       </c>
       <c r="X8" s="1">
-        <f t="shared" ref="X5:X23" si="3">SQRT(LOG(S8)/5.001)</f>
+        <f t="shared" ref="X8:X23" si="9">SQRT(LOG(S8)/5.001)</f>
         <v>0.37387620173887531</v>
       </c>
       <c r="Y8" s="1"/>
@@ -762,54 +798,54 @@
         <v>6.0010000000000003</v>
       </c>
       <c r="B9">
-        <f>T9*$B$1+$E$1</f>
-        <v>0.66451872571274795</v>
+        <f t="shared" si="0"/>
+        <v>0.57634581714183197</v>
       </c>
       <c r="C9">
-        <f>U9*$B$1+$E$1</f>
-        <v>0.58708971624200135</v>
+        <f t="shared" si="2"/>
+        <v>0.52472647749466761</v>
       </c>
       <c r="D9">
-        <f>V9*$B$1+$E$1</f>
-        <v>0.55277083870925625</v>
+        <f t="shared" si="4"/>
+        <v>0.5018472258061708</v>
       </c>
       <c r="E9">
-        <f>W9*$B$1+$E$1</f>
-        <v>0.53230893842987359</v>
+        <f t="shared" si="6"/>
+        <v>0.48820595895324903</v>
       </c>
       <c r="F9">
-        <f>X9*$B$1+$E$1</f>
-        <v>0.5183436700332652</v>
+        <f t="shared" si="8"/>
+        <v>0.47889578002217681</v>
       </c>
       <c r="G9">
-        <f>Y9*$B$1+$E$1</f>
-        <v>0.50803429625184005</v>
+        <f t="shared" ref="G9:G23" si="10">Y9*$B$1+$E$1</f>
+        <v>0.47202286416789341</v>
       </c>
       <c r="S9">
         <v>6.0010000000000003</v>
       </c>
       <c r="T9" s="1">
-        <f>SQRT(LOG(S9)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>0.88172908570915987</v>
       </c>
       <c r="U9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.62363238747333782</v>
       </c>
       <c r="V9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.50923612903085413</v>
       </c>
       <c r="W9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.44102979476624504</v>
       </c>
       <c r="X9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.39447890011088393</v>
       </c>
       <c r="Y9" s="1">
-        <f t="shared" ref="Y5:Y23" si="4">SQRT(LOG(S9)/6.001)</f>
+        <f t="shared" ref="Y9:Y23" si="11">SQRT(LOG(S9)/6.001)</f>
         <v>0.36011432083946682</v>
       </c>
       <c r="Z9" s="1"/>
@@ -823,62 +859,62 @@
         <v>7.0010000000000003</v>
       </c>
       <c r="B10">
-        <f>T10*$B$1+$E$1</f>
-        <v>0.67565996911068726</v>
+        <f t="shared" si="0"/>
+        <v>0.58377331274045818</v>
       </c>
       <c r="C10">
-        <f>U10*$B$1+$E$1</f>
-        <v>0.59496973328157787</v>
+        <f t="shared" si="2"/>
+        <v>0.52997982218771866</v>
       </c>
       <c r="D10">
-        <f>V10*$B$1+$E$1</f>
-        <v>0.55920538164598388</v>
+        <f t="shared" si="4"/>
+        <v>0.50613692109732256</v>
       </c>
       <c r="E10">
-        <f>W10*$B$1+$E$1</f>
-        <v>0.53788164819852313</v>
+        <f t="shared" si="6"/>
+        <v>0.49192109879901547</v>
       </c>
       <c r="F10">
-        <f>X10*$B$1+$E$1</f>
-        <v>0.52332817776100093</v>
+        <f t="shared" si="8"/>
+        <v>0.48221878517400069</v>
       </c>
       <c r="G10">
-        <f>Y10*$B$1+$E$1</f>
-        <v>0.51258458427634046</v>
+        <f t="shared" si="10"/>
+        <v>0.47505638951756035</v>
       </c>
       <c r="H10">
-        <f>Z10*$B$1+$E$1</f>
-        <v>0.5042343117328405</v>
+        <f t="shared" ref="H10:H23" si="12">Z10*$B$1+$E$1</f>
+        <v>0.46948954115522701</v>
       </c>
       <c r="S10">
         <v>7.0010000000000003</v>
       </c>
       <c r="T10" s="1">
-        <f>SQRT(LOG(S10)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>0.9188665637022907</v>
       </c>
       <c r="U10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.64989911093859298</v>
       </c>
       <c r="V10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.53068460548661267</v>
       </c>
       <c r="W10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.45960549399507705</v>
       </c>
       <c r="X10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.41109392587000321</v>
       </c>
       <c r="Y10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.37528194758780153</v>
       </c>
       <c r="Z10" s="1">
-        <f t="shared" ref="Z5:Z23" si="5">SQRT(LOG(S10)/7.001)</f>
+        <f t="shared" ref="Z10:Z23" si="13">SQRT(LOG(S10)/7.001)</f>
         <v>0.34744770577613476</v>
       </c>
       <c r="AA10" s="1"/>
@@ -891,70 +927,70 @@
         <v>8.0009999999999994</v>
       </c>
       <c r="B11">
-        <f>T11*$B$1+$E$1</f>
-        <v>0.68495926472796809</v>
+        <f t="shared" si="0"/>
+        <v>0.58997284315197873</v>
       </c>
       <c r="C11">
-        <f>U11*$B$1+$E$1</f>
-        <v>0.60154697114479405</v>
+        <f t="shared" si="2"/>
+        <v>0.53436464742986267</v>
       </c>
       <c r="D11">
-        <f>V11*$B$1+$E$1</f>
-        <v>0.56457612122984246</v>
+        <f t="shared" si="4"/>
+        <v>0.50971741415322835</v>
       </c>
       <c r="E11">
-        <f>W11*$B$1+$E$1</f>
-        <v>0.54253303886265369</v>
+        <f t="shared" si="6"/>
+        <v>0.49502202590843586</v>
       </c>
       <c r="F11">
-        <f>X11*$B$1+$E$1</f>
-        <v>0.52748861203312269</v>
+        <f t="shared" si="8"/>
+        <v>0.48499240802208177</v>
       </c>
       <c r="G11">
-        <f>Y11*$B$1+$E$1</f>
-        <v>0.51638258706402107</v>
+        <f t="shared" si="10"/>
+        <v>0.47758839137601411</v>
       </c>
       <c r="H11">
-        <f>Z11*$B$1+$E$1</f>
-        <v>0.50775062090676437</v>
+        <f t="shared" si="12"/>
+        <v>0.47183374727117622</v>
       </c>
       <c r="I11">
-        <f>AA11*$B$1+$E$1</f>
-        <v>0.50079237646872421</v>
+        <f t="shared" ref="I11:I23" si="14">AA11*$B$1+$E$1</f>
+        <v>0.46719491764581617</v>
       </c>
       <c r="S11">
         <v>8.0009999999999994</v>
       </c>
       <c r="T11" s="1">
-        <f>SQRT(LOG(S11)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>0.94986421575989344</v>
       </c>
       <c r="U11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.67182323714931325</v>
       </c>
       <c r="V11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.54858707076614155</v>
       </c>
       <c r="W11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.47511012954217913</v>
       </c>
       <c r="X11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.42496204011040883</v>
       </c>
       <c r="Y11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.38794195688007038</v>
       </c>
       <c r="Z11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.35916873635588109</v>
       </c>
       <c r="AA11" s="1">
-        <f t="shared" ref="AA5:AA23" si="6">SQRT(LOG(S11)/8.001)</f>
+        <f t="shared" ref="AA11:AA23" si="15">SQRT(LOG(S11)/8.001)</f>
         <v>0.33597458822908072</v>
       </c>
       <c r="AB11" s="1"/>
@@ -966,78 +1002,78 @@
         <v>9.0009999999999994</v>
       </c>
       <c r="B12">
-        <f>T12*$B$1+$E$1</f>
-        <v>0.69291699879815194</v>
+        <f t="shared" si="0"/>
+        <v>0.595277999198768</v>
       </c>
       <c r="C12">
-        <f>U12*$B$1+$E$1</f>
-        <v>0.60717534473198864</v>
+        <f t="shared" si="2"/>
+        <v>0.53811689648799244</v>
       </c>
       <c r="D12">
-        <f>V12*$B$1+$E$1</f>
-        <v>0.56917205183873021</v>
+        <f t="shared" si="4"/>
+        <v>0.51278136789248685</v>
       </c>
       <c r="E12">
-        <f>W12*$B$1+$E$1</f>
-        <v>0.5465133973204388</v>
+        <f t="shared" si="6"/>
+        <v>0.49767559821362589</v>
       </c>
       <c r="F12">
-        <f>X12*$B$1+$E$1</f>
-        <v>0.53104884185230372</v>
+        <f t="shared" si="8"/>
+        <v>0.48736589456820251</v>
       </c>
       <c r="G12">
-        <f>Y12*$B$1+$E$1</f>
-        <v>0.51963267152482862</v>
+        <f t="shared" si="10"/>
+        <v>0.47975511434988577</v>
       </c>
       <c r="H12">
-        <f>Z12*$B$1+$E$1</f>
-        <v>0.51075965024255998</v>
+        <f t="shared" si="12"/>
+        <v>0.47383976682837337</v>
       </c>
       <c r="I12">
-        <f>AA12*$B$1+$E$1</f>
-        <v>0.50360709080694954</v>
+        <f t="shared" si="14"/>
+        <v>0.46907139387129976</v>
       </c>
       <c r="J12">
-        <f>AB12*$B$1+$E$1</f>
-        <v>0.49768238025224049</v>
+        <f t="shared" ref="J12:J23" si="16">AB12*$B$1+$E$1</f>
+        <v>0.46512158683482702</v>
       </c>
       <c r="S12">
         <v>9.0009999999999994</v>
       </c>
       <c r="T12" s="1">
-        <f>SQRT(LOG(S12)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>0.97638999599383969</v>
       </c>
       <c r="U12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.69058448243996196</v>
       </c>
       <c r="V12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.56390683946243414</v>
       </c>
       <c r="W12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.48837799106812929</v>
       </c>
       <c r="X12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.43682947284101248</v>
       </c>
       <c r="Y12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.39877557174942874</v>
       </c>
       <c r="Z12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.36919883414186672</v>
       </c>
       <c r="AA12" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.34535696935649857</v>
       </c>
       <c r="AB12" s="1">
-        <f t="shared" ref="AB5:AB23" si="7">SQRT(LOG(S12)/9.001)</f>
+        <f t="shared" ref="AB12:AB23" si="17">SQRT(LOG(S12)/9.001)</f>
         <v>0.32560793417413486</v>
       </c>
       <c r="AC12" s="1"/>
@@ -1048,86 +1084,86 @@
         <v>10.000999999999999</v>
       </c>
       <c r="B13">
-        <f>T13*$B$1+$E$1</f>
-        <v>0.69985662317257091</v>
+        <f t="shared" si="0"/>
+        <v>0.59990441544838058</v>
       </c>
       <c r="C13">
-        <f>U13*$B$1+$E$1</f>
-        <v>0.61208362618366186</v>
+        <f t="shared" si="2"/>
+        <v>0.54138908412244124</v>
       </c>
       <c r="D13">
-        <f>V13*$B$1+$E$1</f>
-        <v>0.57317998070331455</v>
+        <f t="shared" si="4"/>
+        <v>0.51545332046887637</v>
       </c>
       <c r="E13" s="2">
-        <f>W13*$B$1+$E$1</f>
-        <v>0.54998451011824701</v>
+        <f t="shared" si="6"/>
+        <v>0.49998967341216471</v>
       </c>
       <c r="F13">
-        <f>X13*$B$1+$E$1</f>
-        <v>0.53415357712164302</v>
+        <f t="shared" si="8"/>
+        <v>0.48943571808109537</v>
       </c>
       <c r="G13">
-        <f>Y13*$B$1+$E$1</f>
-        <v>0.52246694132377147</v>
+        <f t="shared" si="10"/>
+        <v>0.48164462754918097</v>
       </c>
       <c r="H13">
-        <f>Z13*$B$1+$E$1</f>
-        <v>0.51338370542433198</v>
+        <f t="shared" si="12"/>
+        <v>0.47558913694955468</v>
       </c>
       <c r="I13">
-        <f>AA13*$B$1+$E$1</f>
-        <v>0.50606169158354031</v>
+        <f t="shared" si="14"/>
+        <v>0.47070779438902688</v>
       </c>
       <c r="J13">
-        <f>AB13*$B$1+$E$1</f>
-        <v>0.49999661612701413</v>
+        <f t="shared" si="16"/>
+        <v>0.4666644107513428</v>
       </c>
       <c r="K13">
-        <f>AC13*$B$1+$E$1</f>
-        <v>0.49486564655554788</v>
+        <f t="shared" ref="K13:K23" si="18">AC13*$B$1+$E$1</f>
+        <v>0.46324376437036524</v>
       </c>
       <c r="S13">
         <v>10.000999999999999</v>
       </c>
       <c r="T13" s="1">
-        <f>SQRT(LOG(S13)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>0.99952207724190301</v>
       </c>
       <c r="U13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.70694542061220611</v>
       </c>
       <c r="V13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.57726660234438187</v>
       </c>
       <c r="W13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.49994836706082352</v>
       </c>
       <c r="X13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.44717859040547669</v>
       </c>
       <c r="Y13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.40822313774590474</v>
       </c>
       <c r="Z13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.37794568474777335</v>
       </c>
       <c r="AA13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.35353897194513412</v>
       </c>
       <c r="AB13" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.33332205375671375</v>
       </c>
       <c r="AC13" s="1">
-        <f t="shared" ref="AC5:AC23" si="8">SQRT(LOG(S13)/10.001)</f>
+        <f t="shared" ref="AC13:AC23" si="19">SQRT(LOG(S13)/10.001)</f>
         <v>0.31621882185182609</v>
       </c>
       <c r="AD13" s="1"/>
@@ -1137,94 +1173,94 @@
         <v>11.000999999999999</v>
       </c>
       <c r="B14">
-        <f>T14*$B$1+$E$1</f>
-        <v>0.70599879013104316</v>
+        <f t="shared" si="0"/>
+        <v>0.60399919342069552</v>
       </c>
       <c r="C14">
-        <f>U14*$B$1+$E$1</f>
-        <v>0.61642787920497522</v>
+        <f t="shared" si="2"/>
+        <v>0.54428525280331685</v>
       </c>
       <c r="D14">
-        <f>V14*$B$1+$E$1</f>
-        <v>0.57672734392007641</v>
+        <f t="shared" si="4"/>
+        <v>0.51781822928005095</v>
       </c>
       <c r="E14">
-        <f>W14*$B$1+$E$1</f>
-        <v>0.55305674475019906</v>
+        <f t="shared" si="6"/>
+        <v>0.50203782983346601</v>
       </c>
       <c r="F14">
-        <f>X14*$B$1+$E$1</f>
-        <v>0.53690153599625223</v>
+        <f t="shared" si="8"/>
+        <v>0.4912676906641682</v>
       </c>
       <c r="G14">
-        <f>Y14*$B$1+$E$1</f>
-        <v>0.52497551489651895</v>
+        <f t="shared" si="10"/>
+        <v>0.48331700993101268</v>
       </c>
       <c r="H14">
-        <f>Z14*$B$1+$E$1</f>
-        <v>0.51570622090429086</v>
+        <f t="shared" si="12"/>
+        <v>0.4771374806028606</v>
       </c>
       <c r="I14">
-        <f>AA14*$B$1+$E$1</f>
-        <v>0.50823422527884965</v>
+        <f t="shared" si="14"/>
+        <v>0.47215615018589974</v>
       </c>
       <c r="J14">
-        <f>AB14*$B$1+$E$1</f>
-        <v>0.50204491476066115</v>
+        <f t="shared" si="16"/>
+        <v>0.46802994317377411</v>
       </c>
       <c r="K14">
-        <f>AC14*$B$1+$E$1</f>
-        <v>0.49680884405308073</v>
+        <f t="shared" si="18"/>
+        <v>0.4645392293687205</v>
       </c>
       <c r="L14">
-        <f>AD14*$B$1+$E$1</f>
-        <v>0.49230403063549988</v>
+        <f t="shared" ref="L14:L23" si="20">AD14*$B$1+$E$1</f>
+        <v>0.46153602042366659</v>
       </c>
       <c r="S14">
         <v>11.000999999999999</v>
       </c>
       <c r="T14" s="1">
-        <f>SQRT(LOG(S14)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>1.0199959671034773</v>
       </c>
       <c r="U14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.72142626401658405</v>
       </c>
       <c r="V14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.58909114640025451</v>
       </c>
       <c r="W14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.51018914916733016</v>
       </c>
       <c r="X14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.45633845332084078</v>
       </c>
       <c r="Y14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.41658504965506321</v>
       </c>
       <c r="Z14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.38568740301430288</v>
       </c>
       <c r="AA14" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.36078075092949868</v>
       </c>
       <c r="AB14" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.34014971586887044</v>
       </c>
       <c r="AC14" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>0.32269614684360232</v>
       </c>
       <c r="AD14" s="1">
-        <f t="shared" ref="AD5:AI23" si="9">SQRT(LOG(S14)/11.001)</f>
+        <f t="shared" ref="AD14:AD23" si="21">SQRT(LOG(S14)/11.001)</f>
         <v>0.30768010211833297</v>
       </c>
       <c r="AE14" s="1"/>
@@ -1235,102 +1271,102 @@
         <v>12.000999999999999</v>
       </c>
       <c r="B15">
-        <f>T15*$B$1+$E$1</f>
-        <v>0.71150046016099311</v>
+        <f t="shared" si="0"/>
+        <v>0.60766697344066212</v>
       </c>
       <c r="C15">
-        <f>U15*$B$1+$E$1</f>
-        <v>0.6203191193505907</v>
+        <f t="shared" si="2"/>
+        <v>0.54687941290039377</v>
       </c>
       <c r="D15">
-        <f>V15*$B$1+$E$1</f>
-        <v>0.57990479286064689</v>
+        <f t="shared" si="4"/>
+        <v>0.5199365285737646</v>
       </c>
       <c r="E15">
-        <f>W15*$B$1+$E$1</f>
-        <v>0.55580861087722944</v>
+        <f t="shared" si="6"/>
+        <v>0.5038724072514863</v>
       </c>
       <c r="F15">
-        <f>X15*$B$1+$E$1</f>
-        <v>0.53936294140678398</v>
+        <f t="shared" si="8"/>
+        <v>0.49290862760452264</v>
       </c>
       <c r="G15">
-        <f>Y15*$B$1+$E$1</f>
-        <v>0.52722249778324648</v>
+        <f t="shared" si="10"/>
+        <v>0.48481499852216431</v>
       </c>
       <c r="H15">
-        <f>Z15*$B$1+$E$1</f>
-        <v>0.51778654758648235</v>
+        <f t="shared" si="12"/>
+        <v>0.47852436505765494</v>
       </c>
       <c r="I15">
-        <f>AA15*$B$1+$E$1</f>
-        <v>0.51018021007564085</v>
+        <f t="shared" si="14"/>
+        <v>0.47345347338376054</v>
       </c>
       <c r="J15">
-        <f>AB15*$B$1+$E$1</f>
-        <v>0.50387961956131444</v>
+        <f t="shared" si="16"/>
+        <v>0.46925307970754299</v>
       </c>
       <c r="K15">
-        <f>AC15*$B$1+$E$1</f>
-        <v>0.4985494075230632</v>
+        <f t="shared" si="18"/>
+        <v>0.4656996050153755</v>
       </c>
       <c r="L15">
-        <f>AD15*$B$1+$E$1</f>
-        <v>0.49396360033109721</v>
+        <f t="shared" si="20"/>
+        <v>0.4626424002207315</v>
       </c>
       <c r="M15">
-        <f>AE15*$B$1+$E$1</f>
-        <v>0.489963638840403</v>
+        <f t="shared" ref="M15:M23" si="22">AE15*$B$1+$E$1</f>
+        <v>0.45997575922693534</v>
       </c>
       <c r="S15">
         <v>12.000999999999999</v>
       </c>
       <c r="T15" s="1">
-        <f>SQRT(LOG(S15)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>1.0383348672033106</v>
       </c>
       <c r="U15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.73439706450196884</v>
       </c>
       <c r="V15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.599682642868823</v>
       </c>
       <c r="W15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.51936203625743127</v>
       </c>
       <c r="X15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.46454313802261316</v>
       </c>
       <c r="Y15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.42407499261082132</v>
       </c>
       <c r="Z15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.39262182528827444</v>
       </c>
       <c r="AA15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.36726736691880268</v>
       </c>
       <c r="AB15" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.34626539853771487</v>
       </c>
       <c r="AC15" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>0.32849802507687736</v>
       </c>
       <c r="AD15" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>0.31321200110365727</v>
       </c>
       <c r="AE15" s="1">
-        <f t="shared" ref="AE15:AE22" si="10">SQRT(LOG(S15)/12.001)</f>
+        <f t="shared" ref="AE15:AE22" si="23">SQRT(LOG(S15)/12.001)</f>
         <v>0.29987879613467666</v>
       </c>
       <c r="AF15" s="1"/>
@@ -1343,110 +1379,110 @@
         <v>13.000999999999999</v>
       </c>
       <c r="B16">
-        <f>T16*$B$1+$E$1</f>
-        <v>0.71647709316092789</v>
+        <f t="shared" si="0"/>
+        <v>0.61098472877395194</v>
       </c>
       <c r="C16">
-        <f>U16*$B$1+$E$1</f>
-        <v>0.62383900949556836</v>
+        <f t="shared" si="2"/>
+        <v>0.54922600633037888</v>
       </c>
       <c r="D16">
-        <f>V16*$B$1+$E$1</f>
-        <v>0.58277901053767367</v>
+        <f t="shared" si="4"/>
+        <v>0.52185267369178245</v>
       </c>
       <c r="E16">
-        <f>W16*$B$1+$E$1</f>
-        <v>0.55829786008785609</v>
+        <f t="shared" si="6"/>
+        <v>0.5055319067252374</v>
       </c>
       <c r="F16">
-        <f>X16*$B$1+$E$1</f>
-        <v>0.54158944923542252</v>
+        <f t="shared" si="8"/>
+        <v>0.49439296615694833</v>
       </c>
       <c r="G16">
-        <f>Y16*$B$1+$E$1</f>
-        <v>0.5292550459229024</v>
+        <f t="shared" si="10"/>
+        <v>0.48617003061526831</v>
       </c>
       <c r="H16">
-        <f>Z16*$B$1+$E$1</f>
-        <v>0.5196683439066685</v>
+        <f t="shared" si="12"/>
+        <v>0.479778895937779</v>
       </c>
       <c r="I16">
-        <f>AA16*$B$1+$E$1</f>
-        <v>0.51194048506566414</v>
+        <f t="shared" si="14"/>
+        <v>0.47462699004377612</v>
       </c>
       <c r="J16">
-        <f>AB16*$B$1+$E$1</f>
-        <v>0.50553923426128089</v>
+        <f t="shared" si="16"/>
+        <v>0.4703594895075206</v>
       </c>
       <c r="K16">
-        <f>AC16*$B$1+$E$1</f>
-        <v>0.50012386501615902</v>
+        <f t="shared" si="18"/>
+        <v>0.46674924334410606</v>
       </c>
       <c r="L16">
-        <f>AD16*$B$1+$E$1</f>
-        <v>0.49546479347205991</v>
+        <f t="shared" si="20"/>
+        <v>0.46364319564803996</v>
       </c>
       <c r="M16">
-        <f>AE16*$B$1+$E$1</f>
-        <v>0.49140092729132845</v>
+        <f t="shared" si="22"/>
+        <v>0.46093395152755229</v>
       </c>
       <c r="N16">
-        <f>AF16*$B$1+$E$1</f>
-        <v>0.48462131928201796</v>
+        <f t="shared" ref="N16:N23" si="24">AF16*$B$1+$E$1</f>
+        <v>0.45641421285467865</v>
       </c>
       <c r="S16">
         <v>13.000999999999999</v>
       </c>
       <c r="T16" s="1">
-        <f>SQRT(LOG(S16)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>1.0549236438697593</v>
       </c>
       <c r="U16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.74613003165189429</v>
       </c>
       <c r="V16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.60926336845891216</v>
       </c>
       <c r="W16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.52765953362618678</v>
       </c>
       <c r="X16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.47196483078474155</v>
       </c>
       <c r="Y16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.43085015307634134</v>
       </c>
       <c r="Z16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.39889447968889502</v>
       </c>
       <c r="AA16" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.37313495021888055</v>
       </c>
       <c r="AB16" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.35179744753760295</v>
       </c>
       <c r="AC16" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>0.33374621672053018</v>
       </c>
       <c r="AD16" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>0.31821597824019959</v>
       </c>
       <c r="AE16" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0.30466975763776138</v>
       </c>
       <c r="AF16" s="1">
-        <f t="shared" ref="AF15:AF22" si="11">SQRT(LOG(S16)/14.001)</f>
+        <f t="shared" ref="AF16:AF22" si="25">SQRT(LOG(S16)/14.001)</f>
         <v>0.28207106427339318</v>
       </c>
       <c r="AG16" s="1"/>
@@ -1458,118 +1494,118 @@
         <v>14.000999999999999</v>
       </c>
       <c r="B17">
-        <f>T17*$B$1+$E$1</f>
-        <v>0.72101598673694267</v>
+        <f t="shared" si="0"/>
+        <v>0.61401065782462849</v>
       </c>
       <c r="C17">
-        <f>U17*$B$1+$E$1</f>
-        <v>0.62704929379170327</v>
+        <f t="shared" si="2"/>
+        <v>0.55136619586113556</v>
       </c>
       <c r="D17">
-        <f>V17*$B$1+$E$1</f>
-        <v>0.58540041503957219</v>
+        <f t="shared" si="4"/>
+        <v>0.52360027669304809</v>
       </c>
       <c r="E17">
-        <f>W17*$B$1+$E$1</f>
-        <v>0.56056815754627054</v>
+        <f t="shared" si="6"/>
+        <v>0.50704543836418037</v>
       </c>
       <c r="F17">
-        <f>X17*$B$1+$E$1</f>
-        <v>0.54362011576849556</v>
+        <f t="shared" si="8"/>
+        <v>0.4957467438456637</v>
       </c>
       <c r="G17">
-        <f>Y17*$B$1+$E$1</f>
-        <v>0.53110881325799553</v>
+        <f t="shared" si="10"/>
+        <v>0.48740587550533043</v>
       </c>
       <c r="H17">
-        <f>Z17*$B$1+$E$1</f>
-        <v>0.52138461939436742</v>
+        <f t="shared" si="12"/>
+        <v>0.48092307959624497</v>
       </c>
       <c r="I17">
-        <f>AA17*$B$1+$E$1</f>
-        <v>0.51354592811206556</v>
+        <f t="shared" si="14"/>
+        <v>0.47569728540804368</v>
       </c>
       <c r="J17">
-        <f>AB17*$B$1+$E$1</f>
-        <v>0.50705287099126206</v>
+        <f t="shared" si="16"/>
+        <v>0.47136858066084142</v>
       </c>
       <c r="K17">
-        <f>AC17*$B$1+$E$1</f>
-        <v>0.50155983487795419</v>
+        <f t="shared" si="18"/>
+        <v>0.4677065565853028</v>
       </c>
       <c r="L17">
-        <f>AD17*$B$1+$E$1</f>
-        <v>0.49683394323736563</v>
+        <f t="shared" si="20"/>
+        <v>0.46455596215824374</v>
       </c>
       <c r="M17">
-        <f>AE17*$B$1+$E$1</f>
-        <v>0.49271179335617016</v>
+        <f t="shared" si="22"/>
+        <v>0.4618078622374468</v>
       </c>
       <c r="N17">
-        <f>AF17*$B$1+$E$1</f>
-        <v>0.48583495265638593</v>
+        <f t="shared" si="24"/>
+        <v>0.45722330177092396</v>
       </c>
       <c r="O17">
-        <f>AG17*$B$1+$E$1</f>
-        <v>0.48583495265638593</v>
+        <f t="shared" ref="O17:O23" si="26">AG17*$B$1+$E$1</f>
+        <v>0.45722330177092396</v>
       </c>
       <c r="S17">
         <v>14.000999999999999</v>
       </c>
       <c r="T17" s="1">
-        <f>SQRT(LOG(S17)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>1.0700532891231422</v>
       </c>
       <c r="U17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.75683097930567744</v>
       </c>
       <c r="V17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.61800138346524036</v>
       </c>
       <c r="W17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.53522719182090184</v>
       </c>
       <c r="X17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.47873371922831842</v>
       </c>
       <c r="Y17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.43702937752665189</v>
       </c>
       <c r="Z17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.40461539798122481</v>
       </c>
       <c r="AA17" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.3784864270402184</v>
       </c>
       <c r="AB17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.35684290330420687</v>
       </c>
       <c r="AC17" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>0.33853278292651395</v>
       </c>
       <c r="AD17" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>0.32277981079121865</v>
       </c>
       <c r="AE17" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0.30903931118723382</v>
       </c>
       <c r="AF17" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>0.28611650885461964</v>
       </c>
       <c r="AG17" s="1">
-        <f t="shared" ref="AG15:AG22" si="12">SQRT(LOG(S17)/14.001)</f>
+        <f t="shared" ref="AG17:AG22" si="27">SQRT(LOG(S17)/14.001)</f>
         <v>0.28611650885461964</v>
       </c>
       <c r="AH17" s="1"/>
@@ -1580,126 +1616,126 @@
         <v>15.000999999999999</v>
       </c>
       <c r="B18">
-        <f>T18*$B$1+$E$1</f>
-        <v>0.72518467663948538</v>
+        <f t="shared" si="0"/>
+        <v>0.6167897844263236</v>
       </c>
       <c r="C18">
-        <f>U18*$B$1+$E$1</f>
-        <v>0.62999773915739932</v>
+        <f t="shared" si="2"/>
+        <v>0.55333182610493292</v>
       </c>
       <c r="D18">
-        <f>V18*$B$1+$E$1</f>
-        <v>0.58780801114080927</v>
+        <f t="shared" si="4"/>
+        <v>0.5252053407605396</v>
       </c>
       <c r="E18">
-        <f>W18*$B$1+$E$1</f>
-        <v>0.5626532837851127</v>
+        <f t="shared" si="6"/>
+        <v>0.50843552252340851</v>
       </c>
       <c r="F18">
-        <f>X18*$B$1+$E$1</f>
-        <v>0.54548515598811775</v>
+        <f t="shared" si="8"/>
+        <v>0.49699010399207855</v>
       </c>
       <c r="G18">
-        <f>Y18*$B$1+$E$1</f>
-        <v>0.53281138262694983</v>
+        <f t="shared" si="10"/>
+        <v>0.48854092175129993</v>
       </c>
       <c r="H18">
-        <f>Z18*$B$1+$E$1</f>
-        <v>0.52296091109976439</v>
+        <f t="shared" si="12"/>
+        <v>0.48197394073317634</v>
       </c>
       <c r="I18">
-        <f>AA18*$B$1+$E$1</f>
-        <v>0.5150204271512161</v>
+        <f t="shared" si="14"/>
+        <v>0.47668028476747742</v>
       </c>
       <c r="J18">
-        <f>AB18*$B$1+$E$1</f>
-        <v>0.50844305167003667</v>
+        <f t="shared" si="16"/>
+        <v>0.47229536778002446</v>
       </c>
       <c r="K18">
-        <f>AC18*$B$1+$E$1</f>
-        <v>0.50287868339532271</v>
+        <f t="shared" si="18"/>
+        <v>0.46858578893021519</v>
       </c>
       <c r="L18">
-        <f>AD18*$B$1+$E$1</f>
-        <v>0.49809142167481107</v>
+        <f t="shared" si="20"/>
+        <v>0.46539428111654074</v>
       </c>
       <c r="M18">
-        <f>AE18*$B$1+$E$1</f>
-        <v>0.49391574185960463</v>
+        <f t="shared" si="22"/>
+        <v>0.4626104945730698</v>
       </c>
       <c r="N18">
-        <f>AF18*$B$1+$E$1</f>
-        <v>0.4869495990142233</v>
+        <f t="shared" si="24"/>
+        <v>0.45796639934281552</v>
       </c>
       <c r="O18">
-        <f>AG18*$B$1+$E$1</f>
-        <v>0.4869495990142233</v>
+        <f t="shared" si="26"/>
+        <v>0.45796639934281552</v>
       </c>
       <c r="P18">
-        <f>AH18*$B$1+$E$1</f>
-        <v>0.48400149313918894</v>
+        <f t="shared" ref="P18:P23" si="28">AH18*$B$1+$E$1</f>
+        <v>0.45600099542612599</v>
       </c>
       <c r="S18">
         <v>15.000999999999999</v>
       </c>
       <c r="T18" s="1">
-        <f>SQRT(LOG(S18)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>1.0839489221316176</v>
       </c>
       <c r="U18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.76665913052466439</v>
       </c>
       <c r="V18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.62602670380269765</v>
       </c>
       <c r="W18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.54217761261704223</v>
       </c>
       <c r="X18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.48495051996039257</v>
       </c>
       <c r="Y18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.44270460875649942</v>
       </c>
       <c r="Z18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.40986970366588144</v>
       </c>
       <c r="AA18" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.38340142383738696</v>
       </c>
       <c r="AB18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.36147683890012222</v>
       </c>
       <c r="AC18" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>0.34292894465107582</v>
       </c>
       <c r="AD18" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>0.32697140558270354</v>
       </c>
       <c r="AE18" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0.31305247286534871</v>
       </c>
       <c r="AF18" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>0.2898319967140775</v>
       </c>
       <c r="AG18" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>0.2898319967140775</v>
       </c>
       <c r="AH18" s="1">
-        <f t="shared" ref="AH15:AH22" si="13">SQRT(LOG(S18)/15.001)</f>
+        <f t="shared" ref="AH18:AH22" si="29">SQRT(LOG(S18)/15.001)</f>
         <v>0.28000497713062977</v>
       </c>
       <c r="AI18" s="1"/>
@@ -1709,134 +1745,134 @@
         <v>16.001000000000001</v>
       </c>
       <c r="B19">
-        <f>T19*$B$1+$E$1</f>
-        <v>0.72903643611743596</v>
+        <f t="shared" si="0"/>
+        <v>0.61935762407829065</v>
       </c>
       <c r="C19">
-        <f>U19*$B$1+$E$1</f>
-        <v>0.63272202487978246</v>
+        <f t="shared" si="2"/>
+        <v>0.55514801658652169</v>
       </c>
       <c r="D19">
-        <f>V19*$B$1+$E$1</f>
-        <v>0.59003256641328505</v>
+        <f t="shared" si="4"/>
+        <v>0.52668837760885667</v>
       </c>
       <c r="E19">
-        <f>W19*$B$1+$E$1</f>
-        <v>0.56457988541318904</v>
+        <f t="shared" si="6"/>
+        <v>0.5097199236087927</v>
       </c>
       <c r="F19">
-        <f>X19*$B$1+$E$1</f>
-        <v>0.54720840394146342</v>
+        <f t="shared" si="8"/>
+        <v>0.49813893596097564</v>
       </c>
       <c r="G19">
-        <f>Y19*$B$1+$E$1</f>
-        <v>0.53438451180111513</v>
+        <f t="shared" si="10"/>
+        <v>0.48958967453407676</v>
       </c>
       <c r="H19">
-        <f>Z19*$B$1+$E$1</f>
-        <v>0.52441736304467279</v>
+        <f t="shared" si="12"/>
+        <v>0.48294490869644852</v>
       </c>
       <c r="I19">
-        <f>AA19*$B$1+$E$1</f>
-        <v>0.51638282535833946</v>
+        <f t="shared" si="14"/>
+        <v>0.47758855023889302</v>
       </c>
       <c r="J19">
-        <f>AB19*$B$1+$E$1</f>
-        <v>0.50972754193693515</v>
+        <f t="shared" si="16"/>
+        <v>0.47315169462462348</v>
       </c>
       <c r="K19">
-        <f>AC19*$B$1+$E$1</f>
-        <v>0.50409726462720017</v>
+        <f t="shared" si="18"/>
+        <v>0.46939817641813347</v>
       </c>
       <c r="L19">
-        <f>AD19*$B$1+$E$1</f>
-        <v>0.4992532985721056</v>
+        <f t="shared" si="20"/>
+        <v>0.46616886571473709</v>
       </c>
       <c r="M19">
-        <f>AE19*$B$1+$E$1</f>
-        <v>0.4950281585102746</v>
+        <f t="shared" si="22"/>
+        <v>0.46335210567351642</v>
       </c>
       <c r="N19">
-        <f>AF19*$B$1+$E$1</f>
-        <v>0.48797950283862251</v>
+        <f t="shared" si="24"/>
+        <v>0.45865300189241504</v>
       </c>
       <c r="O19">
-        <f>AG19*$B$1+$E$1</f>
-        <v>0.48797950283862251</v>
+        <f t="shared" si="26"/>
+        <v>0.45865300189241504</v>
       </c>
       <c r="P19">
-        <f>AH19*$B$1+$E$1</f>
-        <v>0.48499647713014615</v>
+        <f t="shared" si="28"/>
+        <v>0.45666431808676411</v>
       </c>
       <c r="Q19">
         <f>AI19*$B$1+$E$1</f>
-        <v>0.48229765654503909</v>
+        <v>0.45486510436335942</v>
       </c>
       <c r="S19">
         <v>16.001000000000001</v>
       </c>
       <c r="T19" s="1">
-        <f>SQRT(LOG(S19)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>1.0967881203914529</v>
       </c>
       <c r="U19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.77574008293260821</v>
       </c>
       <c r="V19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.63344188804428325</v>
       </c>
       <c r="W19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.54859961804396329</v>
       </c>
       <c r="X19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.49069467980487802</v>
       </c>
       <c r="Y19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.44794837267038368</v>
       </c>
       <c r="Z19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.41472454348224247</v>
       </c>
       <c r="AA19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.38794275119446481</v>
       </c>
       <c r="AB19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.36575847312311721</v>
       </c>
       <c r="AC19" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>0.34699088209066731</v>
       </c>
       <c r="AD19" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>0.33084432857368523</v>
       </c>
       <c r="AE19" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0.31676052836758195</v>
       </c>
       <c r="AF19" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>0.29326500946207495</v>
       </c>
       <c r="AG19" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>0.29326500946207495</v>
       </c>
       <c r="AH19" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="29"/>
         <v>0.28332159043382038</v>
       </c>
       <c r="AI19" s="1">
-        <f t="shared" ref="AI15:AI22" si="14">SQRT(LOG(S19)/16.001)</f>
+        <f t="shared" ref="AI19:AI22" si="30">SQRT(LOG(S19)/16.001)</f>
         <v>0.27432552181679698</v>
       </c>
     </row>
@@ -1845,134 +1881,134 @@
         <v>17.001000000000001</v>
       </c>
       <c r="B20">
-        <f>T20*$B$1+$E$1</f>
-        <v>0.73261399548502437</v>
+        <f t="shared" si="0"/>
+        <v>0.62174266365668296</v>
       </c>
       <c r="C20">
-        <f>U20*$B$1+$E$1</f>
-        <v>0.63525237340281249</v>
+        <f t="shared" si="2"/>
+        <v>0.55683491560187504</v>
       </c>
       <c r="D20">
-        <f>V20*$B$1+$E$1</f>
-        <v>0.59209875943476564</v>
+        <f t="shared" si="4"/>
+        <v>0.5280658396231771</v>
       </c>
       <c r="E20">
-        <f>W20*$B$1+$E$1</f>
-        <v>0.56636933559604485</v>
+        <f t="shared" si="6"/>
+        <v>0.51091289039736321</v>
       </c>
       <c r="F20">
-        <f>X20*$B$1+$E$1</f>
-        <v>0.54880897684677099</v>
+        <f t="shared" si="8"/>
+        <v>0.49920598456451398</v>
       </c>
       <c r="G20">
-        <f>Y20*$B$1+$E$1</f>
-        <v>0.53584565262407646</v>
+        <f t="shared" si="10"/>
+        <v>0.49056376841605098</v>
       </c>
       <c r="H20">
-        <f>Z20*$B$1+$E$1</f>
-        <v>0.52577013268898121</v>
+        <f t="shared" si="12"/>
+        <v>0.48384675512598752</v>
       </c>
       <c r="I20">
-        <f>AA20*$B$1+$E$1</f>
-        <v>0.51764823678815008</v>
+        <f t="shared" si="14"/>
+        <v>0.47843215785876669</v>
       </c>
       <c r="J20">
-        <f>AB20*$B$1+$E$1</f>
-        <v>0.51092059155834191</v>
+        <f t="shared" si="16"/>
+        <v>0.47394706103889461</v>
       </c>
       <c r="K20">
-        <f>AC20*$B$1+$E$1</f>
-        <v>0.50522909716405173</v>
+        <f t="shared" si="18"/>
+        <v>0.47015273144270114</v>
       </c>
       <c r="L20">
-        <f>AD20*$B$1+$E$1</f>
-        <v>0.50033246345810001</v>
+        <f t="shared" si="20"/>
+        <v>0.46688830897206668</v>
       </c>
       <c r="M20">
-        <f>AE20*$B$1+$E$1</f>
-        <v>0.49606138413924955</v>
+        <f t="shared" si="22"/>
+        <v>0.46404092275949971</v>
       </c>
       <c r="N20">
-        <f>AF20*$B$1+$E$1</f>
-        <v>0.48893608958703888</v>
+        <f t="shared" si="24"/>
+        <v>0.45929072639135926</v>
       </c>
       <c r="O20">
-        <f>AG20*$B$1+$E$1</f>
-        <v>0.48893608958703888</v>
+        <f t="shared" si="26"/>
+        <v>0.45929072639135926</v>
       </c>
       <c r="P20">
-        <f>AH20*$B$1+$E$1</f>
-        <v>0.48592062992780299</v>
+        <f t="shared" si="28"/>
+        <v>0.45728041995186869</v>
       </c>
       <c r="Q20">
         <f>AI20*$B$1+$E$1</f>
-        <v>0.48319246550777117</v>
+        <v>0.45546164367184744</v>
       </c>
       <c r="S20">
         <v>17.001000000000001</v>
       </c>
       <c r="T20" s="1">
-        <f>SQRT(LOG(S20)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>1.1087133182834144</v>
       </c>
       <c r="U20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.78417457800937496</v>
       </c>
       <c r="V20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.64032919811588551</v>
       </c>
       <c r="W20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.55456445198681614</v>
       </c>
       <c r="X20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.49602992282256986</v>
       </c>
       <c r="Y20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.45281884208025464</v>
       </c>
       <c r="Z20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.41923377562993752</v>
       </c>
       <c r="AA20" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.39216078929383336</v>
       </c>
       <c r="AB20" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.36973530519447306</v>
       </c>
       <c r="AC20" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>0.35076365721350561</v>
       </c>
       <c r="AD20" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>0.33444154486033334</v>
       </c>
       <c r="AE20" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0.32020461379749843</v>
       </c>
       <c r="AF20" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>0.29645363195679619</v>
       </c>
       <c r="AG20" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>0.29645363195679619</v>
       </c>
       <c r="AH20" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="29"/>
         <v>0.28640209975934322</v>
       </c>
       <c r="AI20" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="30"/>
         <v>0.27730821835923708</v>
       </c>
     </row>
@@ -1981,134 +2017,134 @@
         <v>18.001000000000001</v>
       </c>
       <c r="B21">
-        <f>T21*$B$1+$E$1</f>
-        <v>0.73595212908739294</v>
+        <f t="shared" si="0"/>
+        <v>0.62396808605826193</v>
       </c>
       <c r="C21">
-        <f>U21*$B$1+$E$1</f>
-        <v>0.63761338004520507</v>
+        <f t="shared" si="2"/>
+        <v>0.55840892003013676</v>
       </c>
       <c r="D21">
-        <f>V21*$B$1+$E$1</f>
-        <v>0.59402667387176167</v>
+        <f t="shared" si="4"/>
+        <v>0.52935111591450779</v>
       </c>
       <c r="E21">
-        <f>W21*$B$1+$E$1</f>
-        <v>0.56803902802359008</v>
+        <f t="shared" si="6"/>
+        <v>0.51202601868239339</v>
       </c>
       <c r="F21">
-        <f>X21*$B$1+$E$1</f>
-        <v>0.55030243248209965</v>
+        <f t="shared" si="8"/>
+        <v>0.50020162165473314</v>
       </c>
       <c r="G21">
-        <f>Y21*$B$1+$E$1</f>
-        <v>0.53720900757580914</v>
+        <f t="shared" si="10"/>
+        <v>0.4914726717172061</v>
       </c>
       <c r="H21">
-        <f>Z21*$B$1+$E$1</f>
-        <v>0.52703236913062956</v>
+        <f t="shared" si="12"/>
+        <v>0.48468824608708638</v>
       </c>
       <c r="I21">
-        <f>AA21*$B$1+$E$1</f>
-        <v>0.51882896140531254</v>
+        <f t="shared" si="14"/>
+        <v>0.4792193076035417</v>
       </c>
       <c r="J21">
-        <f>AB21*$B$1+$E$1</f>
-        <v>0.51203379713267616</v>
+        <f t="shared" si="16"/>
+        <v>0.47468919808845078</v>
       </c>
       <c r="K21">
-        <f>AC21*$B$1+$E$1</f>
-        <v>0.5062851825662249</v>
+        <f t="shared" si="18"/>
+        <v>0.47085678837748324</v>
       </c>
       <c r="L21">
-        <f>AD21*$B$1+$E$1</f>
-        <v>0.50133940595668458</v>
+        <f t="shared" si="20"/>
+        <v>0.46755960397112312</v>
       </c>
       <c r="M21">
-        <f>AE21*$B$1+$E$1</f>
-        <v>0.49702546183483076</v>
+        <f t="shared" si="22"/>
+        <v>0.46468364122322053</v>
       </c>
       <c r="N21">
-        <f>AF21*$B$1+$E$1</f>
-        <v>0.48982865740782716</v>
+        <f t="shared" si="24"/>
+        <v>0.45988577160521815</v>
       </c>
       <c r="O21">
-        <f>AG21*$B$1+$E$1</f>
-        <v>0.48982865740782716</v>
+        <f t="shared" si="26"/>
+        <v>0.45988577160521815</v>
       </c>
       <c r="P21">
-        <f>AH21*$B$1+$E$1</f>
-        <v>0.48678293441826931</v>
+        <f t="shared" si="28"/>
+        <v>0.45785528961217953</v>
       </c>
       <c r="Q21">
         <f>AI21*$B$1+$E$1</f>
-        <v>0.48402738997981692</v>
+        <v>0.45601825998654466</v>
       </c>
       <c r="S21">
         <v>18.001000000000001</v>
       </c>
       <c r="T21" s="1">
-        <f>SQRT(LOG(S21)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>1.1198404302913096</v>
       </c>
       <c r="U21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.79204460015068356</v>
       </c>
       <c r="V21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.64675557957253882</v>
       </c>
       <c r="W21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.56013009341196673</v>
       </c>
       <c r="X21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.50100810827366538</v>
       </c>
       <c r="Y21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.45736335858603039</v>
       </c>
       <c r="Z21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.42344123043543186</v>
       </c>
       <c r="AA21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.39609653801770828</v>
       </c>
       <c r="AB21" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.37344599044225374</v>
       </c>
       <c r="AC21" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>0.35428394188741619</v>
       </c>
       <c r="AD21" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>0.33779801985561536</v>
       </c>
       <c r="AE21" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0.32341820611610245</v>
       </c>
       <c r="AF21" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>0.29942885802609054</v>
       </c>
       <c r="AG21" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>0.29942885802609054</v>
       </c>
       <c r="AH21" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="29"/>
         <v>0.28927644806089758</v>
       </c>
       <c r="AI21" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="30"/>
         <v>0.28009129993272308</v>
       </c>
     </row>
@@ -2117,134 +2153,134 @@
         <v>19.001000000000001</v>
       </c>
       <c r="B22">
-        <f>T22*$B$1+$E$1</f>
-        <v>0.73907949850986032</v>
+        <f t="shared" si="0"/>
+        <v>0.62605299900657352</v>
       </c>
       <c r="C22">
-        <f>U22*$B$1+$E$1</f>
-        <v>0.6398253166718344</v>
+        <f t="shared" si="2"/>
+        <v>0.55988354444788957</v>
       </c>
       <c r="D22">
-        <f>V22*$B$1+$E$1</f>
-        <v>0.59583286301144045</v>
+        <f t="shared" si="4"/>
+        <v>0.53055524200762694</v>
       </c>
       <c r="E22">
-        <f>W22*$B$1+$E$1</f>
-        <v>0.56960329886018124</v>
+        <f t="shared" si="6"/>
+        <v>0.51306886590678746</v>
       </c>
       <c r="F22">
-        <f>X22*$B$1+$E$1</f>
-        <v>0.55170159382316297</v>
+        <f t="shared" si="8"/>
+        <v>0.50113439588210862</v>
       </c>
       <c r="G22">
-        <f>Y22*$B$1+$E$1</f>
-        <v>0.53848628257312892</v>
+        <f t="shared" si="10"/>
+        <v>0.49232418838208603</v>
       </c>
       <c r="H22">
-        <f>Z22*$B$1+$E$1</f>
-        <v>0.52821491007169141</v>
+        <f t="shared" si="12"/>
+        <v>0.48547660671446091</v>
       </c>
       <c r="I22">
-        <f>AA22*$B$1+$E$1</f>
-        <v>0.51993513704233574</v>
+        <f t="shared" si="14"/>
+        <v>0.4799567580282238</v>
       </c>
       <c r="J22">
-        <f>AB22*$B$1+$E$1</f>
-        <v>0.51307671676645672</v>
+        <f t="shared" si="16"/>
+        <v>0.47538447784430454</v>
       </c>
       <c r="K22">
-        <f>AC22*$B$1+$E$1</f>
-        <v>0.50727458850010576</v>
+        <f t="shared" si="18"/>
+        <v>0.47151639233340387</v>
       </c>
       <c r="L22">
-        <f>AD22*$B$1+$E$1</f>
-        <v>0.5022827717878251</v>
+        <f t="shared" si="20"/>
+        <v>0.46818851452521676</v>
       </c>
       <c r="M22">
-        <f>AE22*$B$1+$E$1</f>
-        <v>0.49792866927503154</v>
+        <f t="shared" si="22"/>
+        <v>0.4652857795166877</v>
       </c>
       <c r="N22">
-        <f>AF22*$B$1+$E$1</f>
-        <v>0.49066486998728509</v>
+        <f t="shared" si="24"/>
+        <v>0.46044324665819009</v>
       </c>
       <c r="O22">
-        <f>AG22*$B$1+$E$1</f>
-        <v>0.49066486998728509</v>
+        <f t="shared" si="26"/>
+        <v>0.46044324665819009</v>
       </c>
       <c r="P22">
-        <f>AH22*$B$1+$E$1</f>
-        <v>0.48759079444353226</v>
+        <f t="shared" si="28"/>
+        <v>0.45839386296235485</v>
       </c>
       <c r="Q22">
         <f>AI22*$B$1+$E$1</f>
-        <v>0.48480959871528911</v>
+        <v>0.45653973247685942</v>
       </c>
       <c r="S22">
         <v>19.001000000000001</v>
       </c>
       <c r="T22" s="1">
-        <f>SQRT(LOG(S22)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>1.1302649950328676</v>
       </c>
       <c r="U22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.79941772223944796</v>
       </c>
       <c r="V22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.6527762100381348</v>
       </c>
       <c r="W22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.56534432953393732</v>
       </c>
       <c r="X22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.50567197941054309</v>
       </c>
       <c r="Y22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.46162094191042985</v>
       </c>
       <c r="Z22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.42738303357230456</v>
       </c>
       <c r="AA22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.39978379014111887</v>
       </c>
       <c r="AB22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.37692238922152255</v>
       </c>
       <c r="AC22" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>0.35758196166701911</v>
       </c>
       <c r="AD22" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>0.34094257262608374</v>
       </c>
       <c r="AE22" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0.32642889758343846</v>
       </c>
       <c r="AF22" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="25"/>
         <v>0.30221623329095021</v>
       </c>
       <c r="AG22" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="27"/>
         <v>0.30221623329095021</v>
       </c>
       <c r="AH22" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="29"/>
         <v>0.29196931481177413</v>
       </c>
       <c r="AI22" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="30"/>
         <v>0.28269866238429692</v>
       </c>
     </row>
@@ -2253,114 +2289,114 @@
         <v>20.001000000000001</v>
       </c>
       <c r="B23">
-        <f>T23*$B$1+$E$1</f>
-        <v>0.74201999387442319</v>
+        <f t="shared" si="0"/>
+        <v>0.6280133292496155</v>
       </c>
       <c r="C23">
-        <f>U23*$B$1+$E$1</f>
-        <v>0.64190508037054672</v>
+        <f t="shared" si="2"/>
+        <v>0.56127005358036453</v>
       </c>
       <c r="D23">
-        <f>V23*$B$1+$E$1</f>
-        <v>0.59753112441752632</v>
+        <f t="shared" si="4"/>
+        <v>0.53168741627835092</v>
       </c>
       <c r="E23">
-        <f>W23*$B$1+$E$1</f>
-        <v>0.57107409764425587</v>
+        <f t="shared" si="6"/>
+        <v>0.51404939842950392</v>
       </c>
       <c r="F23">
-        <f>X23*$B$1+$E$1</f>
-        <v>0.55301714912920241</v>
+        <f t="shared" si="8"/>
+        <v>0.50201143275280158</v>
       </c>
       <c r="G23">
-        <f>Y23*$B$1+$E$1</f>
-        <v>0.5396872347797691</v>
+        <f t="shared" si="10"/>
+        <v>0.49312482318651274</v>
       </c>
       <c r="H23">
-        <f>Z23*$B$1+$E$1</f>
-        <v>0.5293267889979919</v>
+        <f t="shared" si="12"/>
+        <v>0.48621785933199463</v>
       </c>
       <c r="I23">
-        <f>AA23*$B$1+$E$1</f>
-        <v>0.52097521382689826</v>
+        <f t="shared" si="14"/>
+        <v>0.48065014255126548</v>
       </c>
       <c r="J23">
-        <f>AB23*$B$1+$E$1</f>
-        <v>0.51405731737178084</v>
+        <f t="shared" si="16"/>
+        <v>0.47603821158118731</v>
       </c>
       <c r="K23">
-        <f>AC23*$B$1+$E$1</f>
-        <v>0.50820487308412288</v>
+        <f t="shared" si="18"/>
+        <v>0.47213658205608189</v>
       </c>
       <c r="L23">
-        <f>AD23*$B$1+$E$1</f>
-        <v>0.50316976736744146</v>
+        <f t="shared" si="20"/>
+        <v>0.46877984491162761</v>
       </c>
       <c r="M23">
-        <f>AE23*$B$1+$E$1</f>
-        <v>0.49877790610393608</v>
+        <f t="shared" si="22"/>
+        <v>0.46585193740262409</v>
       </c>
       <c r="N23">
-        <f>AF23*$B$1+$E$1</f>
-        <v>0.49145111519260692</v>
+        <f t="shared" si="24"/>
+        <v>0.46096741012840464</v>
       </c>
       <c r="O23">
-        <f>AG23*$B$1+$E$1</f>
-        <v>0.49145111519260692</v>
+        <f t="shared" si="26"/>
+        <v>0.46096741012840464</v>
       </c>
       <c r="P23">
-        <f>AH23*$B$1+$E$1</f>
-        <v>0.48835038128429226</v>
+        <f t="shared" si="28"/>
+        <v>0.45890025418952818</v>
       </c>
       <c r="Q23">
         <f>AI23*$B$1+$E$1</f>
-        <v>0.48554506704347966</v>
+        <v>0.45703004469565311</v>
       </c>
       <c r="S23">
         <v>20.001000000000001</v>
       </c>
       <c r="T23" s="1">
-        <f>SQRT(LOG(S23)/1.001)</f>
+        <f t="shared" si="1"/>
         <v>1.1400666462480775</v>
       </c>
       <c r="U23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.80635026790182229</v>
       </c>
       <c r="V23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.65843708139175428</v>
       </c>
       <c r="W23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.57024699214751962</v>
       </c>
       <c r="X23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.51005716376400778</v>
       </c>
       <c r="Y23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0.46562411593256353</v>
       </c>
       <c r="Z23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0.43108929665997298</v>
       </c>
       <c r="AA23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.40325071275632735</v>
       </c>
       <c r="AB23" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>0.38019105790593627</v>
       </c>
       <c r="AC23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="19"/>
         <v>0.36068291028040933</v>
       </c>
       <c r="AD23" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>0.34389922455813798</v>
       </c>
       <c r="AE23" s="1">
@@ -2390,7 +2426,7 @@
       </c>
       <c r="B25">
         <f>B1</f>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -2458,7 +2494,7 @@
       </c>
       <c r="B28">
         <f>T4*$B$25+$E$25</f>
-        <v>-0.29375276499613789</v>
+        <v>-0.29583517666409193</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.35">
@@ -2467,11 +2503,11 @@
       </c>
       <c r="B29">
         <f>T5*$B$25+$E$25</f>
-        <v>-0.13542432493094678</v>
+        <v>-0.19028288328729784</v>
       </c>
       <c r="C29">
         <f>U5*$B$25+$E$25</f>
-        <v>-0.18359834916775761</v>
+        <v>-0.22239889944517172</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.35">
@@ -2479,16 +2515,16 @@
         <v>3.0009999999999999</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30:P47" si="15">T6*$B$25+$E$25</f>
-        <v>-9.2850226744808945E-2</v>
+        <f t="shared" ref="B30:P47" si="31">T6*$B$25+$E$25</f>
+        <v>-0.16190015116320597</v>
       </c>
       <c r="C30">
-        <f t="shared" si="15"/>
-        <v>-0.15348639422981741</v>
+        <f t="shared" si="31"/>
+        <v>-0.20232426281987825</v>
       </c>
       <c r="D30">
-        <f t="shared" si="15"/>
-        <v>-0.18036217657802417</v>
+        <f t="shared" si="31"/>
+        <v>-0.22024145105201609</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.35">
@@ -2496,20 +2532,20 @@
         <v>4.0010000000000003</v>
       </c>
       <c r="B31">
-        <f t="shared" si="15"/>
-        <v>-6.7317751868531589E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.14487850124568771</v>
       </c>
       <c r="C31">
-        <f t="shared" si="15"/>
-        <v>-0.13542769737692936</v>
+        <f t="shared" si="31"/>
+        <v>-0.19028513158461957</v>
       </c>
       <c r="D31">
-        <f t="shared" si="15"/>
-        <v>-0.16561608406354658</v>
+        <f t="shared" si="31"/>
+        <v>-0.21041072270903105</v>
       </c>
       <c r="E31">
-        <f t="shared" si="15"/>
-        <v>-0.1836152670900783</v>
+        <f t="shared" si="31"/>
+        <v>-0.2224101780600522</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.35">
@@ -2517,24 +2553,24 @@
         <v>5.0010000000000003</v>
       </c>
       <c r="B32">
-        <f t="shared" si="15"/>
-        <v>-4.9296460645954443E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.13286430709730296</v>
       </c>
       <c r="C32">
-        <f t="shared" si="15"/>
-        <v>-0.12268153639319701</v>
+        <f t="shared" si="31"/>
+        <v>-0.18178769092879798</v>
       </c>
       <c r="D32">
-        <f t="shared" si="15"/>
-        <v>-0.15520802025907096</v>
+        <f t="shared" si="31"/>
+        <v>-0.20347201350604729</v>
       </c>
       <c r="E32">
-        <f t="shared" si="15"/>
-        <v>-0.17460124396422946</v>
+        <f t="shared" si="31"/>
+        <v>-0.21640082930948629</v>
       </c>
       <c r="F32">
-        <f t="shared" si="15"/>
-        <v>-0.18783713947833741</v>
+        <f t="shared" si="31"/>
+        <v>-0.22522475965222494</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -2542,28 +2578,28 @@
         <v>6.0010000000000003</v>
       </c>
       <c r="B33">
-        <f t="shared" si="15"/>
-        <v>-3.5481274287252063E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.12365418285816801</v>
       </c>
       <c r="C33">
-        <f t="shared" si="15"/>
-        <v>-0.11291028375799864</v>
+        <f t="shared" si="31"/>
+        <v>-0.1752735225053324</v>
       </c>
       <c r="D33">
-        <f t="shared" si="15"/>
-        <v>-0.14722916129074376</v>
+        <f t="shared" si="31"/>
+        <v>-0.19815277419382915</v>
       </c>
       <c r="E33">
-        <f t="shared" si="15"/>
-        <v>-0.16769106157012648</v>
+        <f t="shared" si="31"/>
+        <v>-0.21179404104675098</v>
       </c>
       <c r="F33">
-        <f t="shared" si="15"/>
-        <v>-0.18165632996673481</v>
+        <f t="shared" si="31"/>
+        <v>-0.2211042199778232</v>
       </c>
       <c r="G33">
-        <f t="shared" si="15"/>
-        <v>-0.19196570374815997</v>
+        <f t="shared" si="31"/>
+        <v>-0.2279771358321066</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
@@ -2571,32 +2607,32 @@
         <v>7.0010000000000003</v>
       </c>
       <c r="B34">
-        <f t="shared" si="15"/>
-        <v>-2.4340030889312803E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.11622668725954183</v>
       </c>
       <c r="C34">
-        <f t="shared" si="15"/>
-        <v>-0.10503026671842211</v>
+        <f t="shared" si="31"/>
+        <v>-0.17002017781228138</v>
       </c>
       <c r="D34">
-        <f t="shared" si="15"/>
-        <v>-0.14079461835401619</v>
+        <f t="shared" si="31"/>
+        <v>-0.19386307890267745</v>
       </c>
       <c r="E34">
-        <f t="shared" si="15"/>
-        <v>-0.16211835180147688</v>
+        <f t="shared" si="31"/>
+        <v>-0.20807890120098457</v>
       </c>
       <c r="F34">
-        <f t="shared" si="15"/>
-        <v>-0.17667182223899902</v>
+        <f t="shared" si="31"/>
+        <v>-0.21778121482599933</v>
       </c>
       <c r="G34">
-        <f t="shared" si="15"/>
-        <v>-0.18741541572365955</v>
+        <f t="shared" si="31"/>
+        <v>-0.22494361048243966</v>
       </c>
       <c r="H34">
-        <f t="shared" si="15"/>
-        <v>-0.19576568826715957</v>
+        <f t="shared" si="31"/>
+        <v>-0.23051045884477303</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
@@ -2604,36 +2640,36 @@
         <v>8.0009999999999994</v>
       </c>
       <c r="B35">
-        <f t="shared" si="15"/>
-        <v>-1.504073527203198E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.11002715684802128</v>
       </c>
       <c r="C35">
-        <f t="shared" si="15"/>
-        <v>-9.8453028855206015E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.16563535257013734</v>
       </c>
       <c r="D35">
-        <f t="shared" si="15"/>
-        <v>-0.13542387877015752</v>
+        <f t="shared" si="31"/>
+        <v>-0.19028258584677166</v>
       </c>
       <c r="E35">
-        <f t="shared" si="15"/>
-        <v>-0.15746696113734626</v>
+        <f t="shared" si="31"/>
+        <v>-0.20497797409156415</v>
       </c>
       <c r="F35">
-        <f t="shared" si="15"/>
-        <v>-0.17251138796687734</v>
+        <f t="shared" si="31"/>
+        <v>-0.21500759197791822</v>
       </c>
       <c r="G35">
-        <f t="shared" si="15"/>
-        <v>-0.18361741293597889</v>
+        <f t="shared" si="31"/>
+        <v>-0.2224116086239859</v>
       </c>
       <c r="H35">
-        <f t="shared" si="15"/>
-        <v>-0.19224937909323567</v>
+        <f t="shared" si="31"/>
+        <v>-0.22816625272882377</v>
       </c>
       <c r="I35">
-        <f t="shared" si="15"/>
-        <v>-0.19920762353127577</v>
+        <f t="shared" si="31"/>
+        <v>-0.23280508235418385</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
@@ -2641,40 +2677,40 @@
         <v>9.0009999999999994</v>
       </c>
       <c r="B36">
-        <f t="shared" si="15"/>
-        <v>-7.0830012018480715E-3</v>
+        <f t="shared" si="31"/>
+        <v>-0.10472200080123203</v>
       </c>
       <c r="C36">
-        <f t="shared" si="15"/>
-        <v>-9.2824655268011397E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.1618831035120076</v>
       </c>
       <c r="D36">
-        <f t="shared" si="15"/>
-        <v>-0.13082794816126975</v>
+        <f t="shared" si="31"/>
+        <v>-0.18721863210751316</v>
       </c>
       <c r="E36">
-        <f t="shared" si="15"/>
-        <v>-0.15348660267956121</v>
+        <f t="shared" si="31"/>
+        <v>-0.20232440178637412</v>
       </c>
       <c r="F36">
-        <f t="shared" si="15"/>
-        <v>-0.16895115814769626</v>
+        <f t="shared" si="31"/>
+        <v>-0.2126341054317975</v>
       </c>
       <c r="G36">
-        <f t="shared" si="15"/>
-        <v>-0.18036732847517137</v>
+        <f t="shared" si="31"/>
+        <v>-0.22024488565011424</v>
       </c>
       <c r="H36">
-        <f t="shared" si="15"/>
-        <v>-0.18924034975743997</v>
+        <f t="shared" si="31"/>
+        <v>-0.22616023317162665</v>
       </c>
       <c r="I36">
-        <f t="shared" si="15"/>
-        <v>-0.19639290919305041</v>
+        <f t="shared" si="31"/>
+        <v>-0.23092860612870025</v>
       </c>
       <c r="J36">
-        <f t="shared" si="15"/>
-        <v>-0.20231761974775953</v>
+        <f t="shared" si="31"/>
+        <v>-0.23487841316517299</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -2682,44 +2718,44 @@
         <v>10.000999999999999</v>
       </c>
       <c r="B37" s="2">
-        <f t="shared" si="15"/>
-        <v>-1.4337682742909807E-4</v>
+        <f t="shared" si="31"/>
+        <v>-0.10009558455161938</v>
       </c>
       <c r="C37">
-        <f t="shared" si="15"/>
-        <v>-8.7916373816338156E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.15861091587755877</v>
       </c>
       <c r="D37">
-        <f t="shared" si="15"/>
-        <v>-0.12682001929668543</v>
+        <f t="shared" si="31"/>
+        <v>-0.18454667953112361</v>
       </c>
       <c r="E37">
-        <f t="shared" si="15"/>
-        <v>-0.15001548988175295</v>
+        <f t="shared" si="31"/>
+        <v>-0.2000103265878353</v>
       </c>
       <c r="F37">
-        <f t="shared" si="15"/>
-        <v>-0.16584642287835699</v>
+        <f t="shared" si="31"/>
+        <v>-0.21056428191890464</v>
       </c>
       <c r="G37">
-        <f t="shared" si="15"/>
-        <v>-0.17753305867622857</v>
+        <f t="shared" si="31"/>
+        <v>-0.21835537245081904</v>
       </c>
       <c r="H37">
-        <f t="shared" si="15"/>
-        <v>-0.18661629457566797</v>
+        <f t="shared" si="31"/>
+        <v>-0.22441086305044533</v>
       </c>
       <c r="I37">
-        <f t="shared" si="15"/>
-        <v>-0.19393830841645976</v>
+        <f t="shared" si="31"/>
+        <v>-0.22929220561097316</v>
       </c>
       <c r="J37">
-        <f t="shared" si="15"/>
-        <v>-0.20000338387298588</v>
+        <f t="shared" si="31"/>
+        <v>-0.23333558924865722</v>
       </c>
       <c r="K37">
-        <f t="shared" si="15"/>
-        <v>-0.20513435344445216</v>
+        <f t="shared" si="31"/>
+        <v>-0.23675623562963477</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
@@ -2727,48 +2763,48 @@
         <v>11.000999999999999</v>
       </c>
       <c r="B38">
-        <f t="shared" si="15"/>
-        <v>5.9987901310432079E-3</v>
+        <f t="shared" si="31"/>
+        <v>-9.6000806579304515E-2</v>
       </c>
       <c r="C38">
-        <f t="shared" si="15"/>
-        <v>-8.3572120795024768E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.15571474719668318</v>
       </c>
       <c r="D38">
-        <f t="shared" si="15"/>
-        <v>-0.12327265607992363</v>
+        <f t="shared" si="31"/>
+        <v>-0.18218177071994907</v>
       </c>
       <c r="E38">
-        <f t="shared" si="15"/>
-        <v>-0.14694325524980095</v>
+        <f t="shared" si="31"/>
+        <v>-0.19796217016653395</v>
       </c>
       <c r="F38">
-        <f t="shared" si="15"/>
-        <v>-0.16309846400374775</v>
+        <f t="shared" si="31"/>
+        <v>-0.20873230933583181</v>
       </c>
       <c r="G38">
-        <f t="shared" si="15"/>
-        <v>-0.17502448510348104</v>
+        <f t="shared" si="31"/>
+        <v>-0.21668299006898734</v>
       </c>
       <c r="H38">
-        <f t="shared" si="15"/>
-        <v>-0.18429377909570913</v>
+        <f t="shared" si="31"/>
+        <v>-0.22286251939713941</v>
       </c>
       <c r="I38">
-        <f t="shared" si="15"/>
-        <v>-0.19176577472115039</v>
+        <f t="shared" si="31"/>
+        <v>-0.22784384981410025</v>
       </c>
       <c r="J38">
-        <f t="shared" si="15"/>
-        <v>-0.19795508523933886</v>
+        <f t="shared" si="31"/>
+        <v>-0.2319700568262259</v>
       </c>
       <c r="K38">
-        <f t="shared" si="15"/>
-        <v>-0.20319115594691928</v>
+        <f t="shared" si="31"/>
+        <v>-0.23546077063127951</v>
       </c>
       <c r="L38">
-        <f t="shared" si="15"/>
-        <v>-0.2076959693645001</v>
+        <f t="shared" si="31"/>
+        <v>-0.23846397957633339</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
@@ -2776,52 +2812,52 @@
         <v>12.000999999999999</v>
       </c>
       <c r="B39">
-        <f t="shared" si="15"/>
-        <v>1.1500460160993153E-2</v>
+        <f t="shared" si="31"/>
+        <v>-9.2333026559337866E-2</v>
       </c>
       <c r="C39">
-        <f t="shared" si="15"/>
-        <v>-7.9680880649409341E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.15312058709960621</v>
       </c>
       <c r="D39">
-        <f t="shared" si="15"/>
-        <v>-0.12009520713935309</v>
+        <f t="shared" si="31"/>
+        <v>-0.18006347142623538</v>
       </c>
       <c r="E39">
-        <f t="shared" si="15"/>
-        <v>-0.1441913891227706</v>
+        <f t="shared" si="31"/>
+        <v>-0.19612759274851371</v>
       </c>
       <c r="F39">
-        <f t="shared" si="15"/>
-        <v>-0.16063705859321606</v>
+        <f t="shared" si="31"/>
+        <v>-0.20709137239547737</v>
       </c>
       <c r="G39">
-        <f t="shared" si="15"/>
-        <v>-0.17277750221675359</v>
+        <f t="shared" si="31"/>
+        <v>-0.2151850014778357</v>
       </c>
       <c r="H39">
-        <f t="shared" si="15"/>
-        <v>-0.18221345241351766</v>
+        <f t="shared" si="31"/>
+        <v>-0.2214756349423451</v>
       </c>
       <c r="I39">
-        <f t="shared" si="15"/>
-        <v>-0.18981978992435919</v>
+        <f t="shared" si="31"/>
+        <v>-0.22654652661623945</v>
       </c>
       <c r="J39">
-        <f t="shared" si="15"/>
-        <v>-0.19612038043868552</v>
+        <f t="shared" si="31"/>
+        <v>-0.23074692029245703</v>
       </c>
       <c r="K39">
-        <f t="shared" si="15"/>
-        <v>-0.20145059247693678</v>
+        <f t="shared" si="31"/>
+        <v>-0.23430039498462452</v>
       </c>
       <c r="L39">
-        <f t="shared" si="15"/>
-        <v>-0.2060363996689028</v>
+        <f t="shared" si="31"/>
+        <v>-0.23735759977926851</v>
       </c>
       <c r="M39">
-        <f t="shared" si="15"/>
-        <v>-0.21003636115959701</v>
+        <f t="shared" si="31"/>
+        <v>-0.24002424077306467</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
@@ -2829,56 +2865,56 @@
         <v>13.000999999999999</v>
       </c>
       <c r="B40">
-        <f t="shared" si="15"/>
-        <v>1.6477093160927825E-2</v>
+        <f t="shared" si="31"/>
+        <v>-8.9015271226048104E-2</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40:N40" si="16">U16*$B$25+$E$25</f>
-        <v>-7.6160990504431703E-2</v>
+        <f t="shared" ref="C40:N40" si="32">U16*$B$25+$E$25</f>
+        <v>-0.15077399366962113</v>
       </c>
       <c r="D40">
-        <f t="shared" si="16"/>
-        <v>-0.11722098946232634</v>
+        <f t="shared" si="32"/>
+        <v>-0.17814732630821756</v>
       </c>
       <c r="E40">
-        <f t="shared" si="16"/>
-        <v>-0.14170213991214395</v>
+        <f t="shared" si="32"/>
+        <v>-0.19446809327476261</v>
       </c>
       <c r="F40">
-        <f t="shared" si="16"/>
-        <v>-0.15841055076457752</v>
+        <f t="shared" si="32"/>
+        <v>-0.20560703384305168</v>
       </c>
       <c r="G40">
-        <f t="shared" si="16"/>
-        <v>-0.17074495407709758</v>
+        <f t="shared" si="32"/>
+        <v>-0.2138299693847317</v>
       </c>
       <c r="H40">
-        <f t="shared" si="16"/>
-        <v>-0.18033165609333149</v>
+        <f t="shared" si="32"/>
+        <v>-0.22022110406222098</v>
       </c>
       <c r="I40">
-        <f t="shared" si="16"/>
-        <v>-0.18805951493433581</v>
+        <f t="shared" si="32"/>
+        <v>-0.22537300995622389</v>
       </c>
       <c r="J40">
-        <f t="shared" si="16"/>
-        <v>-0.19446076573871912</v>
+        <f t="shared" si="32"/>
+        <v>-0.22964051049247941</v>
       </c>
       <c r="K40">
-        <f t="shared" si="16"/>
-        <v>-0.19987613498384094</v>
+        <f t="shared" si="32"/>
+        <v>-0.23325075665589395</v>
       </c>
       <c r="L40">
-        <f t="shared" si="16"/>
-        <v>-0.20453520652794011</v>
+        <f t="shared" si="32"/>
+        <v>-0.23635680435196005</v>
       </c>
       <c r="M40">
-        <f t="shared" si="16"/>
-        <v>-0.20859907270867156</v>
+        <f t="shared" si="32"/>
+        <v>-0.23906604847244772</v>
       </c>
       <c r="N40">
-        <f t="shared" si="16"/>
-        <v>-0.21537868071798205</v>
+        <f t="shared" si="32"/>
+        <v>-0.24358578714532136</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
@@ -2886,60 +2922,60 @@
         <v>14.000999999999999</v>
       </c>
       <c r="B41">
-        <f t="shared" si="15"/>
-        <v>2.101598673694266E-2</v>
+        <f t="shared" si="31"/>
+        <v>-8.5989342175371519E-2</v>
       </c>
       <c r="C41">
-        <f t="shared" si="15"/>
-        <v>-7.2950706208296773E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.14863380413886448</v>
       </c>
       <c r="D41">
-        <f t="shared" si="15"/>
-        <v>-0.11459958496042788</v>
+        <f t="shared" si="31"/>
+        <v>-0.17639972330695192</v>
       </c>
       <c r="E41">
-        <f t="shared" si="15"/>
-        <v>-0.13943184245372944</v>
+        <f t="shared" si="31"/>
+        <v>-0.19295456163581962</v>
       </c>
       <c r="F41">
-        <f t="shared" si="15"/>
-        <v>-0.15637988423150448</v>
+        <f t="shared" si="31"/>
+        <v>-0.20425325615433632</v>
       </c>
       <c r="G41">
-        <f t="shared" si="15"/>
-        <v>-0.16889118674200443</v>
+        <f t="shared" si="31"/>
+        <v>-0.21259412449466961</v>
       </c>
       <c r="H41">
-        <f t="shared" si="15"/>
-        <v>-0.17861538060563253</v>
+        <f t="shared" si="31"/>
+        <v>-0.21907692040375504</v>
       </c>
       <c r="I41">
-        <f t="shared" si="15"/>
-        <v>-0.18645407188793447</v>
+        <f t="shared" si="31"/>
+        <v>-0.2243027145919563</v>
       </c>
       <c r="J41">
-        <f t="shared" si="15"/>
-        <v>-0.19294712900873795</v>
+        <f t="shared" si="31"/>
+        <v>-0.22863141933915859</v>
       </c>
       <c r="K41">
-        <f t="shared" si="15"/>
-        <v>-0.19844016512204582</v>
+        <f t="shared" si="31"/>
+        <v>-0.23229344341469721</v>
       </c>
       <c r="L41">
-        <f t="shared" si="15"/>
-        <v>-0.20316605676263438</v>
+        <f t="shared" si="31"/>
+        <v>-0.23544403784175627</v>
       </c>
       <c r="M41">
-        <f t="shared" si="15"/>
-        <v>-0.20728820664382985</v>
+        <f t="shared" si="31"/>
+        <v>-0.23819213776255321</v>
       </c>
       <c r="N41">
-        <f t="shared" si="15"/>
-        <v>-0.21416504734361408</v>
+        <f t="shared" si="31"/>
+        <v>-0.24277669822907605</v>
       </c>
       <c r="O41">
-        <f t="shared" si="15"/>
-        <v>-0.21416504734361408</v>
+        <f t="shared" si="31"/>
+        <v>-0.24277669822907605</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
@@ -2947,64 +2983,64 @@
         <v>15.000999999999999</v>
       </c>
       <c r="B42">
-        <f t="shared" si="15"/>
-        <v>2.5184676639485315E-2</v>
+        <f t="shared" si="31"/>
+        <v>-8.3210215573676444E-2</v>
       </c>
       <c r="C42">
-        <f t="shared" ref="C42:P42" si="17">U18*$B$25+$E$25</f>
-        <v>-7.0002260842600694E-2</v>
+        <f t="shared" ref="C42:P42" si="33">U18*$B$25+$E$25</f>
+        <v>-0.14666817389506709</v>
       </c>
       <c r="D42">
-        <f t="shared" si="17"/>
-        <v>-0.11219198885919071</v>
+        <f t="shared" si="33"/>
+        <v>-0.17479465923946044</v>
       </c>
       <c r="E42">
-        <f t="shared" si="17"/>
-        <v>-0.13734671621488734</v>
+        <f t="shared" si="33"/>
+        <v>-0.19156447747659155</v>
       </c>
       <c r="F42">
-        <f t="shared" si="17"/>
-        <v>-0.15451484401188223</v>
+        <f t="shared" si="33"/>
+        <v>-0.20300989600792146</v>
       </c>
       <c r="G42">
-        <f t="shared" si="17"/>
-        <v>-0.16718861737305016</v>
+        <f t="shared" si="33"/>
+        <v>-0.21145907824870008</v>
       </c>
       <c r="H42">
-        <f t="shared" si="17"/>
-        <v>-0.17703908890023556</v>
+        <f t="shared" si="33"/>
+        <v>-0.2180260592668237</v>
       </c>
       <c r="I42">
-        <f t="shared" si="17"/>
-        <v>-0.18497957284878391</v>
+        <f t="shared" si="33"/>
+        <v>-0.22331971523252259</v>
       </c>
       <c r="J42">
-        <f t="shared" si="17"/>
-        <v>-0.19155694832996334</v>
+        <f t="shared" si="33"/>
+        <v>-0.22770463221997556</v>
       </c>
       <c r="K42">
-        <f t="shared" si="17"/>
-        <v>-0.19712131660467724</v>
+        <f t="shared" si="33"/>
+        <v>-0.23141421106978483</v>
       </c>
       <c r="L42">
-        <f t="shared" si="17"/>
-        <v>-0.20190857832518894</v>
+        <f t="shared" si="33"/>
+        <v>-0.23460571888345927</v>
       </c>
       <c r="M42">
-        <f t="shared" si="17"/>
-        <v>-0.20608425814039538</v>
+        <f t="shared" si="33"/>
+        <v>-0.23738950542693024</v>
       </c>
       <c r="N42">
-        <f t="shared" si="17"/>
-        <v>-0.21305040098577674</v>
+        <f t="shared" si="33"/>
+        <v>-0.24203360065718449</v>
       </c>
       <c r="O42">
-        <f t="shared" si="17"/>
-        <v>-0.21305040098577674</v>
+        <f t="shared" si="33"/>
+        <v>-0.24203360065718449</v>
       </c>
       <c r="P42">
-        <f t="shared" si="17"/>
-        <v>-0.21599850686081107</v>
+        <f t="shared" si="33"/>
+        <v>-0.24399900457387402</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
@@ -3012,68 +3048,68 @@
         <v>16.001000000000001</v>
       </c>
       <c r="B43">
-        <f t="shared" si="15"/>
-        <v>2.9036436117435893E-2</v>
+        <f t="shared" si="31"/>
+        <v>-8.0642375921709392E-2</v>
       </c>
       <c r="C43">
-        <f t="shared" si="15"/>
-        <v>-6.7277975120217548E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.14485198341347832</v>
       </c>
       <c r="D43">
-        <f t="shared" si="15"/>
-        <v>-0.10996743358671501</v>
+        <f t="shared" si="31"/>
+        <v>-0.17331162239114334</v>
       </c>
       <c r="E43">
-        <f t="shared" si="15"/>
-        <v>-0.135420114586811</v>
+        <f t="shared" si="31"/>
+        <v>-0.19028007639120731</v>
       </c>
       <c r="F43">
-        <f t="shared" si="15"/>
-        <v>-0.15279159605853659</v>
+        <f t="shared" si="31"/>
+        <v>-0.20186106403902437</v>
       </c>
       <c r="G43">
-        <f t="shared" si="15"/>
-        <v>-0.16561548819888489</v>
+        <f t="shared" si="31"/>
+        <v>-0.21041032546592325</v>
       </c>
       <c r="H43">
-        <f t="shared" si="15"/>
-        <v>-0.17558263695532725</v>
+        <f t="shared" si="31"/>
+        <v>-0.2170550913035515</v>
       </c>
       <c r="I43">
-        <f t="shared" si="15"/>
-        <v>-0.18361717464166055</v>
+        <f t="shared" si="31"/>
+        <v>-0.22241144976110702</v>
       </c>
       <c r="J43">
-        <f t="shared" si="15"/>
-        <v>-0.19027245806306481</v>
+        <f t="shared" si="31"/>
+        <v>-0.22684830537537654</v>
       </c>
       <c r="K43">
-        <f t="shared" si="15"/>
-        <v>-0.19590273537279979</v>
+        <f t="shared" si="31"/>
+        <v>-0.23060182358186654</v>
       </c>
       <c r="L43">
-        <f t="shared" si="15"/>
-        <v>-0.20074670142789441</v>
+        <f t="shared" si="31"/>
+        <v>-0.23383113428526292</v>
       </c>
       <c r="M43">
-        <f t="shared" si="15"/>
-        <v>-0.20497184148972541</v>
+        <f t="shared" si="31"/>
+        <v>-0.23664789432648359</v>
       </c>
       <c r="N43">
-        <f t="shared" si="15"/>
-        <v>-0.2120204971613775</v>
+        <f t="shared" si="31"/>
+        <v>-0.241346998107585</v>
       </c>
       <c r="O43">
-        <f t="shared" si="15"/>
-        <v>-0.2120204971613775</v>
+        <f t="shared" si="31"/>
+        <v>-0.241346998107585</v>
       </c>
       <c r="P43">
-        <f t="shared" si="15"/>
-        <v>-0.21500352286985386</v>
+        <f t="shared" si="31"/>
+        <v>-0.2433356819132359</v>
       </c>
       <c r="Q43">
-        <f t="shared" ref="Q43:Q46" si="18">AI19*$B$25+$E$25</f>
-        <v>-0.21770234345496089</v>
+        <f t="shared" ref="Q43:Q46" si="34">AI19*$B$25+$E$25</f>
+        <v>-0.24513489563664059</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
@@ -3081,68 +3117,68 @@
         <v>17.001000000000001</v>
       </c>
       <c r="B44">
-        <f t="shared" si="15"/>
-        <v>3.2613995485024305E-2</v>
+        <f t="shared" si="31"/>
+        <v>-7.8257336343317108E-2</v>
       </c>
       <c r="C44">
-        <f t="shared" si="15"/>
-        <v>-6.4747626597187524E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.14316508439812498</v>
       </c>
       <c r="D44">
-        <f t="shared" si="15"/>
-        <v>-0.10790124056523434</v>
+        <f t="shared" si="31"/>
+        <v>-0.17193416037682288</v>
       </c>
       <c r="E44">
-        <f t="shared" si="15"/>
-        <v>-0.13363066440395516</v>
+        <f t="shared" si="31"/>
+        <v>-0.18908710960263675</v>
       </c>
       <c r="F44">
-        <f t="shared" si="15"/>
-        <v>-0.15119102315322905</v>
+        <f t="shared" si="31"/>
+        <v>-0.20079401543548603</v>
       </c>
       <c r="G44">
-        <f t="shared" si="15"/>
-        <v>-0.1641543473759236</v>
+        <f t="shared" si="31"/>
+        <v>-0.20943623158394906</v>
       </c>
       <c r="H44">
-        <f t="shared" si="15"/>
-        <v>-0.17422986731101875</v>
+        <f t="shared" si="31"/>
+        <v>-0.2161532448740125</v>
       </c>
       <c r="I44">
-        <f t="shared" si="15"/>
-        <v>-0.18235176321184998</v>
+        <f t="shared" si="31"/>
+        <v>-0.22156784214123332</v>
       </c>
       <c r="J44">
-        <f t="shared" si="15"/>
-        <v>-0.18907940844165808</v>
+        <f t="shared" si="31"/>
+        <v>-0.22605293896110537</v>
       </c>
       <c r="K44">
-        <f t="shared" si="15"/>
-        <v>-0.19477090283594831</v>
+        <f t="shared" si="31"/>
+        <v>-0.22984726855729887</v>
       </c>
       <c r="L44">
-        <f t="shared" si="15"/>
-        <v>-0.1996675365419</v>
+        <f t="shared" si="31"/>
+        <v>-0.23311169102793333</v>
       </c>
       <c r="M44">
-        <f t="shared" si="15"/>
-        <v>-0.20393861586075046</v>
+        <f t="shared" si="31"/>
+        <v>-0.2359590772405003</v>
       </c>
       <c r="N44">
-        <f t="shared" si="15"/>
-        <v>-0.21106391041296113</v>
+        <f t="shared" si="31"/>
+        <v>-0.24070927360864075</v>
       </c>
       <c r="O44">
-        <f t="shared" si="15"/>
-        <v>-0.21106391041296113</v>
+        <f t="shared" si="31"/>
+        <v>-0.24070927360864075</v>
       </c>
       <c r="P44">
-        <f t="shared" si="15"/>
-        <v>-0.21407937007219702</v>
+        <f t="shared" si="31"/>
+        <v>-0.24271958004813135</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="18"/>
-        <v>-0.21680753449222886</v>
+        <f t="shared" si="34"/>
+        <v>-0.24453835632815257</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
@@ -3150,68 +3186,68 @@
         <v>18.001000000000001</v>
       </c>
       <c r="B45">
-        <f t="shared" si="15"/>
-        <v>3.595212908739287E-2</v>
+        <f t="shared" si="31"/>
+        <v>-7.6031913941738055E-2</v>
       </c>
       <c r="C45">
-        <f t="shared" si="15"/>
-        <v>-6.2386619954794942E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.14159107996986325</v>
       </c>
       <c r="D45">
-        <f t="shared" si="15"/>
-        <v>-0.10597332612823834</v>
+        <f t="shared" si="31"/>
+        <v>-0.17064888408549223</v>
       </c>
       <c r="E45">
-        <f t="shared" si="15"/>
-        <v>-0.13196097197640996</v>
+        <f t="shared" si="31"/>
+        <v>-0.18797398131760662</v>
       </c>
       <c r="F45">
-        <f t="shared" si="15"/>
-        <v>-0.14969756751790039</v>
+        <f t="shared" si="31"/>
+        <v>-0.19979837834526692</v>
       </c>
       <c r="G45">
-        <f t="shared" si="15"/>
-        <v>-0.16279099242419087</v>
+        <f t="shared" si="31"/>
+        <v>-0.20852732828279391</v>
       </c>
       <c r="H45">
-        <f t="shared" si="15"/>
-        <v>-0.17296763086937045</v>
+        <f t="shared" si="31"/>
+        <v>-0.21531175391291363</v>
       </c>
       <c r="I45">
-        <f t="shared" si="15"/>
-        <v>-0.18117103859468753</v>
+        <f t="shared" si="31"/>
+        <v>-0.22078069239645831</v>
       </c>
       <c r="J45">
-        <f t="shared" si="15"/>
-        <v>-0.18796620286732385</v>
+        <f t="shared" si="31"/>
+        <v>-0.22531080191154923</v>
       </c>
       <c r="K45">
-        <f t="shared" si="15"/>
-        <v>-0.19371481743377514</v>
+        <f t="shared" si="31"/>
+        <v>-0.22914321162251675</v>
       </c>
       <c r="L45">
-        <f t="shared" si="15"/>
-        <v>-0.19866059404331537</v>
+        <f t="shared" si="31"/>
+        <v>-0.23244039602887689</v>
       </c>
       <c r="M45">
-        <f t="shared" si="15"/>
-        <v>-0.20297453816516925</v>
+        <f t="shared" si="31"/>
+        <v>-0.23531635877677948</v>
       </c>
       <c r="N45">
-        <f t="shared" si="15"/>
-        <v>-0.21017134259217285</v>
+        <f t="shared" si="31"/>
+        <v>-0.24011422839478189</v>
       </c>
       <c r="O45">
-        <f t="shared" si="15"/>
-        <v>-0.21017134259217285</v>
+        <f t="shared" si="31"/>
+        <v>-0.24011422839478189</v>
       </c>
       <c r="P45">
-        <f t="shared" si="15"/>
-        <v>-0.2132170655817307</v>
+        <f t="shared" si="31"/>
+        <v>-0.24214471038782048</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="18"/>
-        <v>-0.21597261002018309</v>
+        <f t="shared" si="34"/>
+        <v>-0.24398174001345538</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
@@ -3219,68 +3255,68 @@
         <v>19.001000000000001</v>
       </c>
       <c r="B46">
-        <f t="shared" si="15"/>
-        <v>3.9079498509860255E-2</v>
+        <f t="shared" si="31"/>
+        <v>-7.3947000993426465E-2</v>
       </c>
       <c r="C46">
-        <f t="shared" si="15"/>
-        <v>-6.0174683328165612E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.14011645555211039</v>
       </c>
       <c r="D46">
-        <f t="shared" si="15"/>
-        <v>-0.10416713698855956</v>
+        <f t="shared" si="31"/>
+        <v>-0.16944475799237302</v>
       </c>
       <c r="E46">
-        <f t="shared" si="15"/>
-        <v>-0.1303967011398188</v>
+        <f t="shared" si="31"/>
+        <v>-0.18693113409321252</v>
       </c>
       <c r="F46">
-        <f t="shared" si="15"/>
-        <v>-0.14829840617683707</v>
+        <f t="shared" si="31"/>
+        <v>-0.19886560411789136</v>
       </c>
       <c r="G46">
-        <f t="shared" si="15"/>
-        <v>-0.16151371742687104</v>
+        <f t="shared" si="31"/>
+        <v>-0.20767581161791401</v>
       </c>
       <c r="H46">
-        <f t="shared" si="15"/>
-        <v>-0.17178508992830863</v>
+        <f t="shared" si="31"/>
+        <v>-0.21452339328553907</v>
       </c>
       <c r="I46">
-        <f t="shared" si="15"/>
-        <v>-0.18006486295766433</v>
+        <f t="shared" si="31"/>
+        <v>-0.22004324197177622</v>
       </c>
       <c r="J46">
-        <f t="shared" si="15"/>
-        <v>-0.18692328323354324</v>
+        <f t="shared" si="31"/>
+        <v>-0.22461552215569547</v>
       </c>
       <c r="K46">
-        <f t="shared" si="15"/>
-        <v>-0.19272541149989425</v>
+        <f t="shared" si="31"/>
+        <v>-0.22848360766659614</v>
       </c>
       <c r="L46">
-        <f t="shared" si="15"/>
-        <v>-0.19771722821217486</v>
+        <f t="shared" si="31"/>
+        <v>-0.23181148547478325</v>
       </c>
       <c r="M46">
-        <f t="shared" si="15"/>
-        <v>-0.20207133072496847</v>
+        <f t="shared" si="31"/>
+        <v>-0.23471422048331231</v>
       </c>
       <c r="N46">
-        <f t="shared" si="15"/>
-        <v>-0.20933513001271492</v>
+        <f t="shared" si="31"/>
+        <v>-0.23955675334180995</v>
       </c>
       <c r="O46">
-        <f t="shared" si="15"/>
-        <v>-0.20933513001271492</v>
+        <f t="shared" si="31"/>
+        <v>-0.23955675334180995</v>
       </c>
       <c r="P46">
-        <f t="shared" si="15"/>
-        <v>-0.21240920555646775</v>
+        <f t="shared" si="31"/>
+        <v>-0.24160613703764516</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="18"/>
-        <v>-0.2151904012847109</v>
+        <f t="shared" si="34"/>
+        <v>-0.24346026752314059</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
@@ -3288,71 +3324,968 @@
         <v>20.001000000000001</v>
       </c>
       <c r="B47">
-        <f t="shared" si="15"/>
-        <v>4.2019993874423234E-2</v>
+        <f t="shared" si="31"/>
+        <v>-7.1986670750384479E-2</v>
       </c>
       <c r="C47">
-        <f t="shared" si="15"/>
-        <v>-5.8094919629453318E-2</v>
+        <f t="shared" si="31"/>
+        <v>-0.13872994641963551</v>
       </c>
       <c r="D47">
-        <f t="shared" si="15"/>
-        <v>-0.10246887558247372</v>
+        <f t="shared" si="31"/>
+        <v>-0.16831258372164912</v>
       </c>
       <c r="E47">
-        <f t="shared" si="15"/>
-        <v>-0.12892590235574411</v>
+        <f t="shared" si="31"/>
+        <v>-0.18595060157049606</v>
       </c>
       <c r="F47">
-        <f t="shared" si="15"/>
-        <v>-0.14698285087079765</v>
+        <f t="shared" si="31"/>
+        <v>-0.19798856724719843</v>
       </c>
       <c r="G47">
-        <f t="shared" si="15"/>
-        <v>-0.16031276522023094</v>
+        <f t="shared" si="31"/>
+        <v>-0.20687517681348727</v>
       </c>
       <c r="H47">
-        <f t="shared" si="15"/>
-        <v>-0.17067321100200811</v>
+        <f t="shared" si="31"/>
+        <v>-0.21378214066800538</v>
       </c>
       <c r="I47">
-        <f t="shared" si="15"/>
-        <v>-0.1790247861731018</v>
+        <f t="shared" si="31"/>
+        <v>-0.21934985744873453</v>
       </c>
       <c r="J47">
-        <f t="shared" si="15"/>
-        <v>-0.18594268262821911</v>
+        <f t="shared" si="31"/>
+        <v>-0.22396178841881273</v>
       </c>
       <c r="K47">
-        <f t="shared" si="15"/>
-        <v>-0.19179512691587719</v>
+        <f t="shared" si="31"/>
+        <v>-0.22786341794391812</v>
       </c>
       <c r="L47">
-        <f t="shared" si="15"/>
-        <v>-0.19683023263255861</v>
+        <f t="shared" si="31"/>
+        <v>-0.2312201550883724</v>
       </c>
       <c r="M47">
-        <f t="shared" si="15"/>
-        <v>-0.20122209389606394</v>
+        <f t="shared" si="31"/>
+        <v>-0.23414806259737594</v>
       </c>
       <c r="N47">
-        <f t="shared" si="15"/>
-        <v>-0.20854888480739309</v>
+        <f t="shared" si="31"/>
+        <v>-0.2390325898715954</v>
       </c>
       <c r="O47">
-        <f t="shared" si="15"/>
-        <v>-0.20854888480739309</v>
+        <f t="shared" si="31"/>
+        <v>-0.2390325898715954</v>
       </c>
       <c r="P47">
-        <f t="shared" si="15"/>
-        <v>-0.21164961871570775</v>
+        <f t="shared" si="31"/>
+        <v>-0.24109974581047183</v>
       </c>
       <c r="Q47">
-        <f t="shared" ref="Q47" si="19">AI23*$B$25+$E$25</f>
-        <v>-0.21445493295652032</v>
+        <f t="shared" ref="Q47" si="35">AI23*$B$25+$E$25</f>
+        <v>-0.24296995530434687</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <f>SUM(B2)/A2</f>
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <f>-B2+$I$3</f>
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <f>MAX($D$2:D2)</f>
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <f>E2-D2</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <f>F2&gt;$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <f>SUM($B$2:B3)/A3</f>
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <f>D2+(C3-B3+$I$3)</f>
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <f>MAX($D$2:D3)</f>
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F31" si="0">E3-D3</f>
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <f t="shared" ref="G3:G31" si="1">F3&gt;$J$3</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <f>SUM($B$2:B4)/A4</f>
+        <v>-1</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D20" si="2">D3+(C4-B4+$I$3)</f>
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <f>MAX($D$2:D4)</f>
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-1</v>
+      </c>
+      <c r="C5">
+        <f>SUM($B$2:B5)/A5</f>
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <f>MAX($D$2:D5)</f>
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <f>SUM($B$2:B6)/A6</f>
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <f>MAX($D$2:D6)</f>
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-1</v>
+      </c>
+      <c r="C7">
+        <f>SUM($B$2:B7)/A7</f>
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <f>MAX($D$2:D7)</f>
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f>SUM($B$2:B8)/A8</f>
+        <v>-0.7142857142857143</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>6.2857142857142856</v>
+      </c>
+      <c r="E8">
+        <f>MAX($D$2:D8)</f>
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.71428571428571441</v>
+      </c>
+      <c r="G8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
+      <c r="C9">
+        <f>SUM($B$2:B9)/A9</f>
+        <v>-0.75</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>7.5357142857142856</v>
+      </c>
+      <c r="E9">
+        <f>MAX($D$2:D9)</f>
+        <v>7.5357142857142856</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-1</v>
+      </c>
+      <c r="C10">
+        <f>SUM($B$2:B10)/A10</f>
+        <v>-0.77777777777777779</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>8.7579365079365079</v>
+      </c>
+      <c r="E10">
+        <f>MAX($D$2:D10)</f>
+        <v>8.7579365079365079</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-1</v>
+      </c>
+      <c r="C11">
+        <f>SUM($B$2:B11)/A11</f>
+        <v>-0.8</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>9.9579365079365072</v>
+      </c>
+      <c r="E11">
+        <f>MAX($D$2:D11)</f>
+        <v>9.9579365079365072</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f>SUM($B$2:B12)/A12</f>
+        <v>-0.63636363636363635</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>9.3215728715728705</v>
+      </c>
+      <c r="E12">
+        <f>MAX($D$2:D12)</f>
+        <v>9.9579365079365072</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.63636363636363669</v>
+      </c>
+      <c r="G12" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>-1</v>
+      </c>
+      <c r="C13">
+        <f>SUM($B$2:B13)/A13</f>
+        <v>-0.66666666666666663</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>10.654906204906204</v>
+      </c>
+      <c r="E13">
+        <f>MAX($D$2:D13)</f>
+        <v>10.654906204906204</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>-1</v>
+      </c>
+      <c r="C14">
+        <f>SUM($B$2:B14)/A14</f>
+        <v>-0.69230769230769229</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>11.962598512598513</v>
+      </c>
+      <c r="E14">
+        <f>MAX($D$2:D14)</f>
+        <v>11.962598512598513</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>-1</v>
+      </c>
+      <c r="C15">
+        <f>SUM($B$2:B15)/A15</f>
+        <v>-0.7142857142857143</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>13.248312798312799</v>
+      </c>
+      <c r="E15">
+        <f>MAX($D$2:D15)</f>
+        <v>13.248312798312799</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>-1</v>
+      </c>
+      <c r="C16">
+        <f>SUM($B$2:B16)/A16</f>
+        <v>-0.73333333333333328</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>14.514979464979465</v>
+      </c>
+      <c r="E16">
+        <f>MAX($D$2:D16)</f>
+        <v>14.514979464979465</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>-1</v>
+      </c>
+      <c r="C17">
+        <f>SUM($B$2:B17)/A17</f>
+        <v>-0.75</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>15.764979464979465</v>
+      </c>
+      <c r="E17">
+        <f>MAX($D$2:D17)</f>
+        <v>15.764979464979465</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <f>SUM($B$2:B18)/A18</f>
+        <v>-0.6470588235294118</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>15.117920641450054</v>
+      </c>
+      <c r="E18">
+        <f>MAX($D$2:D18)</f>
+        <v>15.764979464979465</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0.64705882352941124</v>
+      </c>
+      <c r="G18" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <f>SUM($B$2:B19)/A19</f>
+        <v>-0.55555555555555558</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>14.562365085894498</v>
+      </c>
+      <c r="E19">
+        <f>MAX($D$2:D19)</f>
+        <v>15.764979464979465</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>1.2026143790849666</v>
+      </c>
+      <c r="G19" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>-1</v>
+      </c>
+      <c r="C20">
+        <f>SUM($B$2:B20)/A20</f>
+        <v>-0.57894736842105265</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>15.983417717473445</v>
+      </c>
+      <c r="E20">
+        <f>MAX($D$2:D20)</f>
+        <v>15.983417717473445</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>-1</v>
+      </c>
+      <c r="C21">
+        <f>SUM($B$2:B21)/A21</f>
+        <v>-0.6</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D31" si="3">D20+(C21-B21+$I$3)</f>
+        <v>17.383417717473446</v>
+      </c>
+      <c r="E21">
+        <f>MAX($D$2:D21)</f>
+        <v>17.383417717473446</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>-1</v>
+      </c>
+      <c r="C22">
+        <f>SUM($B$2:B22)/A22</f>
+        <v>-0.61904761904761907</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="3"/>
+        <v>18.764370098425825</v>
+      </c>
+      <c r="E22">
+        <f>MAX($D$2:D22)</f>
+        <v>18.764370098425825</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>-1</v>
+      </c>
+      <c r="C23">
+        <f>SUM($B$2:B23)/A23</f>
+        <v>-0.63636363636363635</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="3"/>
+        <v>20.128006462062189</v>
+      </c>
+      <c r="E23">
+        <f>MAX($D$2:D23)</f>
+        <v>20.128006462062189</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <f>SUM($B$2:B24)/A24</f>
+        <v>-0.56521739130434778</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="3"/>
+        <v>19.562789070757841</v>
+      </c>
+      <c r="E24">
+        <f>MAX($D$2:D24)</f>
+        <v>20.128006462062189</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0.56521739130434767</v>
+      </c>
+      <c r="G24" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f>SUM($B$2:B25)/A25</f>
+        <v>-0.5</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="3"/>
+        <v>19.062789070757841</v>
+      </c>
+      <c r="E25">
+        <f>MAX($D$2:D25)</f>
+        <v>20.128006462062189</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>1.0652173913043477</v>
+      </c>
+      <c r="G25" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f>SUM($B$2:B26)/A26</f>
+        <v>-0.44</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="3"/>
+        <v>18.62278907075784</v>
+      </c>
+      <c r="E26">
+        <f>MAX($D$2:D26)</f>
+        <v>20.128006462062189</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>1.505217391304349</v>
+      </c>
+      <c r="G26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f>SUM($B$2:B27)/A27</f>
+        <v>-0.38461538461538464</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="3"/>
+        <v>18.238173686142456</v>
+      </c>
+      <c r="E27">
+        <f>MAX($D$2:D27)</f>
+        <v>20.128006462062189</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>1.8898327759197322</v>
+      </c>
+      <c r="G27" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f>SUM($B$2:B28)/A28</f>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="3"/>
+        <v>17.904840352809124</v>
+      </c>
+      <c r="E28">
+        <f>MAX($D$2:D28)</f>
+        <v>20.128006462062189</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>2.2231661092530643</v>
+      </c>
+      <c r="G28" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <f>SUM($B$2:B29)/A29</f>
+        <v>-0.2857142857142857</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>17.61912606709484</v>
+      </c>
+      <c r="E29">
+        <f>MAX($D$2:D29)</f>
+        <v>20.128006462062189</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>2.508880394967349</v>
+      </c>
+      <c r="G29" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <f>SUM($B$2:B30)/A30</f>
+        <v>-0.2413793103448276</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>17.37774675675001</v>
+      </c>
+      <c r="E30">
+        <f>MAX($D$2:D30)</f>
+        <v>20.128006462062189</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>2.7502597053121782</v>
+      </c>
+      <c r="G30" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f>SUM($B$2:B31)/A31</f>
+        <v>-0.2</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>17.177746756750011</v>
+      </c>
+      <c r="E31">
+        <f>MAX($D$2:D31)</f>
+        <v>20.128006462062189</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>2.9502597053121775</v>
+      </c>
+      <c r="G31" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G2:G31">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",G2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>